<commit_message>
13 july 2023 DSR
</commit_message>
<xml_diff>
--- a/07_july_2023/July2023.xlsx
+++ b/07_july_2023/July2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="111">
   <si>
     <t>Day</t>
   </si>
@@ -205,7 +205,7 @@
     <t>work on the coupon category and coupon validation and locale validations and others</t>
   </si>
   <si>
-    <t xml:space="preserve">2h 40m </t>
+    <t xml:space="preserve">2h 50m </t>
   </si>
   <si>
     <t>wbx-4956</t>
@@ -214,13 +214,139 @@
     <t>wbx team meeting with binod</t>
   </si>
   <si>
-    <t xml:space="preserve">1h 25m </t>
+    <t xml:space="preserve">1h 15m </t>
   </si>
   <si>
     <t>rebase the branch and update the code and merged code</t>
   </si>
   <si>
     <t xml:space="preserve">25m </t>
+  </si>
+  <si>
+    <t>wbx-4928</t>
+  </si>
+  <si>
+    <t>check profile image issue on admin side and merchant side test local and dev server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45m </t>
+  </si>
+  <si>
+    <t>15m</t>
+  </si>
+  <si>
+    <t>wbx-4952</t>
+  </si>
+  <si>
+    <t>work on the referral amount update button should be disable at page loading starts</t>
+  </si>
+  <si>
+    <t>work on validations of tracker type store categories  and check every module</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>work on edit profile module where delelete button should be work N delete image showing default image</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>Birthday Celebration of Vimal Sir</t>
+  </si>
+  <si>
+    <t>work on the edit profile validation all fields on admin side N merchant side</t>
+  </si>
+  <si>
+    <t>WBX-4928</t>
+  </si>
+  <si>
+    <t>delete button should be work on merchant side profile image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2h 15m </t>
+  </si>
+  <si>
+    <t>verify the work and raised the pr</t>
+  </si>
+  <si>
+    <t>check every module validation and test some modules and update code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify all the scenario and raised the pr </t>
+  </si>
+  <si>
+    <t>raised the pr N add anull check browser tracker</t>
+  </si>
+  <si>
+    <t>wbx-4719</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test the issue but this issue does not occure again </t>
+  </si>
+  <si>
+    <t>reviewed prs</t>
+  </si>
+  <si>
+    <t>merchand side edit profile validation issue work on the login module validations N test every modules</t>
+  </si>
+  <si>
+    <t>8m</t>
+  </si>
+  <si>
+    <t>update the pr and rebased and merged</t>
+  </si>
+  <si>
+    <t>22m</t>
+  </si>
+  <si>
+    <t>solve git small git comments and update pr  and merged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reviewed pr </t>
+  </si>
+  <si>
+    <t>20m</t>
+  </si>
+  <si>
+    <t>wbx-5016</t>
+  </si>
+  <si>
+    <t>work on the touched validation of user module community module and test every module while create and edit no issue</t>
+  </si>
+  <si>
+    <t>1h 40m</t>
+  </si>
+  <si>
+    <t>work on the touched validation of program and Challenge module and test all this module while create and edit no issue</t>
+  </si>
+  <si>
+    <t>work on the touched validation of achievements module and annoucement module and test both module no error occure white create and edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2h 30m </t>
+  </si>
+  <si>
+    <t>work on the map form and challenge categories touched validation and goal add edit form</t>
+  </si>
+  <si>
+    <t>achievement module and subgoal form validations and locale module custom fields</t>
+  </si>
+  <si>
+    <t>wbx-5029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add team to challenge form and add team form and special sale form </t>
+  </si>
+  <si>
+    <t>notification tracker add edit modules  N tracker type N activities N tracker formula and tracker chart and test while create N edit do not occure any type of error in all modules</t>
+  </si>
+  <si>
+    <t>unit, unit-type</t>
+  </si>
+  <si>
+    <t>pending- coupon,-category, store,-category, merchant.ts, signup, login</t>
   </si>
 </sst>
 </file>
@@ -228,13 +354,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="dd/mmm/yy"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="mmm/yy"/>
-    <numFmt numFmtId="181" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="182" formatCode="h:mm"/>
+    <numFmt numFmtId="176" formatCode="h:mm"/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="181" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="182" formatCode="mmm/yy"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -275,14 +401,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -290,8 +408,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -299,7 +432,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,18 +452,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -358,36 +484,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -404,8 +500,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -444,7 +570,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,13 +606,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -480,13 +636,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,31 +654,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,7 +684,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,60 +727,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -783,17 +909,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -822,25 +966,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -857,33 +992,30 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -892,145 +1024,139 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1048,7 +1174,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="4" borderId="4" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="4" borderId="4" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="4" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1060,7 +1186,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="4" borderId="7" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="4" borderId="7" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="4" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1072,7 +1198,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="4" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="4" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="4" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1085,22 +1211,22 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="5" borderId="12" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="5" borderId="12" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1126,6 +1252,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="1" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1445,10 +1577,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:P74"/>
+  <dimension ref="A2:P143"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="I76" sqref="I76"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="O137" sqref="O137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2707,7 +2839,7 @@
         <v>0.0833333333333333</v>
       </c>
       <c r="E70" s="25">
-        <v>0.194444444444444</v>
+        <v>0.201388888888889</v>
       </c>
       <c r="F70" s="26" t="s">
         <v>62</v>
@@ -2731,7 +2863,7 @@
         <v>64</v>
       </c>
       <c r="D71" s="25">
-        <v>0.194444444444444</v>
+        <v>0.201388888888889</v>
       </c>
       <c r="E71" s="25">
         <v>0.253472222222222</v>
@@ -2810,8 +2942,1275 @@
       <c r="M74" s="34"/>
       <c r="N74" s="34"/>
     </row>
+    <row r="75" spans="1:15">
+      <c r="A75" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="3"/>
+      <c r="O75" s="3"/>
+    </row>
+    <row r="76" spans="1:15">
+      <c r="A76" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" s="7">
+        <v>45115</v>
+      </c>
+      <c r="C76" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="35"/>
+      <c r="E76" s="35"/>
+      <c r="F76" s="35"/>
+      <c r="G76" s="35"/>
+      <c r="H76" s="35"/>
+      <c r="I76" s="35"/>
+      <c r="J76" s="35"/>
+      <c r="K76" s="35"/>
+      <c r="L76" s="35"/>
+      <c r="M76" s="35"/>
+      <c r="N76" s="35"/>
+      <c r="O76" s="35"/>
+    </row>
+    <row r="77" spans="1:15">
+      <c r="A77" s="10"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="35"/>
+      <c r="D77" s="35"/>
+      <c r="E77" s="35"/>
+      <c r="F77" s="35"/>
+      <c r="G77" s="35"/>
+      <c r="H77" s="35"/>
+      <c r="I77" s="35"/>
+      <c r="J77" s="35"/>
+      <c r="K77" s="35"/>
+      <c r="L77" s="35"/>
+      <c r="M77" s="35"/>
+      <c r="N77" s="35"/>
+      <c r="O77" s="35"/>
+    </row>
+    <row r="78" spans="1:15">
+      <c r="A78" s="14"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="35"/>
+      <c r="D78" s="35"/>
+      <c r="E78" s="35"/>
+      <c r="F78" s="35"/>
+      <c r="G78" s="35"/>
+      <c r="H78" s="35"/>
+      <c r="I78" s="35"/>
+      <c r="J78" s="35"/>
+      <c r="K78" s="35"/>
+      <c r="L78" s="35"/>
+      <c r="M78" s="35"/>
+      <c r="N78" s="35"/>
+      <c r="O78" s="35"/>
+    </row>
+    <row r="79" spans="1:14">
+      <c r="A79" s="18"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="18"/>
+      <c r="E79" s="18"/>
+      <c r="F79" s="18"/>
+      <c r="G79" s="18"/>
+      <c r="H79" s="18"/>
+      <c r="I79" s="18"/>
+      <c r="J79" s="18"/>
+      <c r="K79" s="18"/>
+      <c r="L79" s="18"/>
+      <c r="M79" s="18"/>
+      <c r="N79" s="18"/>
+    </row>
+    <row r="80" spans="1:14">
+      <c r="A80" s="18"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="18"/>
+      <c r="E80" s="18"/>
+      <c r="F80" s="18"/>
+      <c r="G80" s="18"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
+      <c r="J80" s="18"/>
+      <c r="K80" s="18"/>
+      <c r="L80" s="18"/>
+      <c r="M80" s="18"/>
+      <c r="N80" s="18"/>
+    </row>
+    <row r="81" spans="1:15">
+      <c r="A81" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
+      <c r="M81" s="3"/>
+      <c r="N81" s="3"/>
+      <c r="O81" s="3"/>
+    </row>
+    <row r="82" spans="1:15">
+      <c r="A82" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="7">
+        <v>45116</v>
+      </c>
+      <c r="C82" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" s="35"/>
+      <c r="E82" s="35"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="35"/>
+      <c r="H82" s="35"/>
+      <c r="I82" s="35"/>
+      <c r="J82" s="35"/>
+      <c r="K82" s="35"/>
+      <c r="L82" s="35"/>
+      <c r="M82" s="35"/>
+      <c r="N82" s="35"/>
+      <c r="O82" s="35"/>
+    </row>
+    <row r="83" spans="1:15">
+      <c r="A83" s="10"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="35"/>
+      <c r="D83" s="35"/>
+      <c r="E83" s="35"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="35"/>
+      <c r="H83" s="35"/>
+      <c r="I83" s="35"/>
+      <c r="J83" s="35"/>
+      <c r="K83" s="35"/>
+      <c r="L83" s="35"/>
+      <c r="M83" s="35"/>
+      <c r="N83" s="35"/>
+      <c r="O83" s="35"/>
+    </row>
+    <row r="84" spans="1:15">
+      <c r="A84" s="14"/>
+      <c r="B84" s="15"/>
+      <c r="C84" s="35"/>
+      <c r="D84" s="35"/>
+      <c r="E84" s="35"/>
+      <c r="F84" s="35"/>
+      <c r="G84" s="35"/>
+      <c r="H84" s="35"/>
+      <c r="I84" s="35"/>
+      <c r="J84" s="35"/>
+      <c r="K84" s="35"/>
+      <c r="L84" s="35"/>
+      <c r="M84" s="35"/>
+      <c r="N84" s="35"/>
+      <c r="O84" s="35"/>
+    </row>
+    <row r="87" spans="1:15">
+      <c r="A87" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B87" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E87" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F87" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G87" s="19"/>
+      <c r="H87" s="19"/>
+      <c r="I87" s="19"/>
+      <c r="J87" s="19"/>
+      <c r="K87" s="19"/>
+      <c r="L87" s="19"/>
+      <c r="M87" s="19"/>
+      <c r="N87" s="19"/>
+      <c r="O87" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
+      <c r="A88" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B88" s="20">
+        <v>45117</v>
+      </c>
+      <c r="C88" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D88" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E88" s="25">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="F88" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G88" s="23"/>
+      <c r="H88" s="23"/>
+      <c r="I88" s="23"/>
+      <c r="J88" s="23"/>
+      <c r="K88" s="23"/>
+      <c r="L88" s="23"/>
+      <c r="M88" s="23"/>
+      <c r="N88" s="23"/>
+      <c r="O88" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
+      <c r="A89" s="20"/>
+      <c r="B89" s="20"/>
+      <c r="C89" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D89" s="25">
+        <v>0.427083333333333</v>
+      </c>
+      <c r="E89" s="25">
+        <v>0.4375</v>
+      </c>
+      <c r="F89" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G89" s="23"/>
+      <c r="H89" s="23"/>
+      <c r="I89" s="23"/>
+      <c r="J89" s="23"/>
+      <c r="K89" s="23"/>
+      <c r="L89" s="23"/>
+      <c r="M89" s="23"/>
+      <c r="N89" s="23"/>
+      <c r="O89" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15">
+      <c r="A90" s="20"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D90" s="25">
+        <v>0.4375</v>
+      </c>
+      <c r="E90" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F90" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="G90" s="26"/>
+      <c r="H90" s="26"/>
+      <c r="I90" s="26"/>
+      <c r="J90" s="26"/>
+      <c r="K90" s="26"/>
+      <c r="L90" s="26"/>
+      <c r="M90" s="26"/>
+      <c r="N90" s="26"/>
+      <c r="O90" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
+      <c r="A91" s="20"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D91" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E91" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F91" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="G91" s="26"/>
+      <c r="H91" s="26"/>
+      <c r="I91" s="26"/>
+      <c r="J91" s="26"/>
+      <c r="K91" s="26"/>
+      <c r="L91" s="26"/>
+      <c r="M91" s="26"/>
+      <c r="N91" s="26"/>
+      <c r="O91" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15">
+      <c r="A92" s="20"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D92" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E92" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F92" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G92" s="26"/>
+      <c r="H92" s="26"/>
+      <c r="I92" s="26"/>
+      <c r="J92" s="26"/>
+      <c r="K92" s="26"/>
+      <c r="L92" s="26"/>
+      <c r="M92" s="26"/>
+      <c r="N92" s="26"/>
+      <c r="O92" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15">
+      <c r="A93" s="20"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="36"/>
+      <c r="D93" s="25"/>
+      <c r="E93" s="25"/>
+      <c r="F93" s="26"/>
+      <c r="G93" s="26"/>
+      <c r="H93" s="26"/>
+      <c r="I93" s="26"/>
+      <c r="J93" s="26"/>
+      <c r="K93" s="26"/>
+      <c r="L93" s="26"/>
+      <c r="M93" s="26"/>
+      <c r="N93" s="26"/>
+      <c r="O93" s="25"/>
+    </row>
+    <row r="94" spans="1:15">
+      <c r="A94" s="20"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D94" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E94" s="25">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="F94" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G94" s="26"/>
+      <c r="H94" s="26"/>
+      <c r="I94" s="26"/>
+      <c r="J94" s="26"/>
+      <c r="K94" s="26"/>
+      <c r="L94" s="26"/>
+      <c r="M94" s="26"/>
+      <c r="N94" s="26"/>
+      <c r="O94" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15">
+      <c r="A95" s="20"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D95" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E95" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F95" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="G95" s="26"/>
+      <c r="H95" s="26"/>
+      <c r="I95" s="26"/>
+      <c r="J95" s="26"/>
+      <c r="K95" s="26"/>
+      <c r="L95" s="26"/>
+      <c r="M95" s="26"/>
+      <c r="N95" s="26"/>
+      <c r="O95" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15">
+      <c r="A99" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B99" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F99" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G99" s="19"/>
+      <c r="H99" s="19"/>
+      <c r="I99" s="19"/>
+      <c r="J99" s="19"/>
+      <c r="K99" s="19"/>
+      <c r="L99" s="19"/>
+      <c r="M99" s="19"/>
+      <c r="N99" s="19"/>
+      <c r="O99" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15">
+      <c r="A100" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B100" s="20">
+        <v>45118</v>
+      </c>
+      <c r="C100" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D100" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E100" s="22">
+        <v>0.40625</v>
+      </c>
+      <c r="F100" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G100" s="23"/>
+      <c r="H100" s="23"/>
+      <c r="I100" s="23"/>
+      <c r="J100" s="23"/>
+      <c r="K100" s="23"/>
+      <c r="L100" s="23"/>
+      <c r="M100" s="23"/>
+      <c r="N100" s="23"/>
+      <c r="O100" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15">
+      <c r="A101" s="20"/>
+      <c r="B101" s="20"/>
+      <c r="C101" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D101" s="22">
+        <v>0.40625</v>
+      </c>
+      <c r="E101" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F101" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="G101" s="23"/>
+      <c r="H101" s="23"/>
+      <c r="I101" s="23"/>
+      <c r="J101" s="23"/>
+      <c r="K101" s="23"/>
+      <c r="L101" s="23"/>
+      <c r="M101" s="23"/>
+      <c r="N101" s="23"/>
+      <c r="O101" s="25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15">
+      <c r="A102" s="20"/>
+      <c r="B102" s="20"/>
+      <c r="C102" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D102" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E102" s="25">
+        <v>0.520833333333333</v>
+      </c>
+      <c r="F102" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="G102" s="26"/>
+      <c r="H102" s="26"/>
+      <c r="I102" s="26"/>
+      <c r="J102" s="26"/>
+      <c r="K102" s="26"/>
+      <c r="L102" s="26"/>
+      <c r="M102" s="26"/>
+      <c r="N102" s="26"/>
+      <c r="O102" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15">
+      <c r="A103" s="20"/>
+      <c r="B103" s="20"/>
+      <c r="C103" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D103" s="25">
+        <v>0.520833333333333</v>
+      </c>
+      <c r="E103" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F103" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G103" s="26"/>
+      <c r="H103" s="26"/>
+      <c r="I103" s="26"/>
+      <c r="J103" s="26"/>
+      <c r="K103" s="26"/>
+      <c r="L103" s="26"/>
+      <c r="M103" s="26"/>
+      <c r="N103" s="26"/>
+      <c r="O103" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15">
+      <c r="A104" s="20"/>
+      <c r="B104" s="20"/>
+      <c r="C104" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D104" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E104" s="25">
+        <v>0.125</v>
+      </c>
+      <c r="F104" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G104" s="26"/>
+      <c r="H104" s="26"/>
+      <c r="I104" s="26"/>
+      <c r="J104" s="26"/>
+      <c r="K104" s="26"/>
+      <c r="L104" s="26"/>
+      <c r="M104" s="26"/>
+      <c r="N104" s="26"/>
+      <c r="O104" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15">
+      <c r="A105" s="20"/>
+      <c r="B105" s="20"/>
+      <c r="C105" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D105" s="25">
+        <v>0.125</v>
+      </c>
+      <c r="E105" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F105" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="G105" s="26"/>
+      <c r="H105" s="26"/>
+      <c r="I105" s="26"/>
+      <c r="J105" s="26"/>
+      <c r="K105" s="26"/>
+      <c r="L105" s="26"/>
+      <c r="M105" s="26"/>
+      <c r="N105" s="26"/>
+      <c r="O105" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15">
+      <c r="A106" s="20"/>
+      <c r="B106" s="20"/>
+      <c r="C106" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D106" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E106" s="25">
+        <v>0.1875</v>
+      </c>
+      <c r="F106" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="G106" s="26"/>
+      <c r="H106" s="26"/>
+      <c r="I106" s="26"/>
+      <c r="J106" s="26"/>
+      <c r="K106" s="26"/>
+      <c r="L106" s="26"/>
+      <c r="M106" s="26"/>
+      <c r="N106" s="26"/>
+      <c r="O106" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15">
+      <c r="A107" s="20"/>
+      <c r="B107" s="20"/>
+      <c r="C107" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D107" s="25">
+        <v>0.1875</v>
+      </c>
+      <c r="E107" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="F107" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="G107" s="26"/>
+      <c r="H107" s="26"/>
+      <c r="I107" s="26"/>
+      <c r="J107" s="26"/>
+      <c r="K107" s="26"/>
+      <c r="L107" s="26"/>
+      <c r="M107" s="26"/>
+      <c r="N107" s="26"/>
+      <c r="O107" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15">
+      <c r="A108" s="20"/>
+      <c r="B108" s="20"/>
+      <c r="C108" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D108" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E108" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F108" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="G108" s="26"/>
+      <c r="H108" s="26"/>
+      <c r="I108" s="26"/>
+      <c r="J108" s="26"/>
+      <c r="K108" s="26"/>
+      <c r="L108" s="26"/>
+      <c r="M108" s="26"/>
+      <c r="N108" s="26"/>
+      <c r="O108" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15">
+      <c r="A112" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B112" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D112" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F112" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G112" s="19"/>
+      <c r="H112" s="19"/>
+      <c r="I112" s="19"/>
+      <c r="J112" s="19"/>
+      <c r="K112" s="19"/>
+      <c r="L112" s="19"/>
+      <c r="M112" s="19"/>
+      <c r="N112" s="19"/>
+      <c r="O112" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15">
+      <c r="A113" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B113" s="20">
+        <v>45119</v>
+      </c>
+      <c r="C113" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D113" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E113" s="22">
+        <v>0.401388888888889</v>
+      </c>
+      <c r="F113" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G113" s="23"/>
+      <c r="H113" s="23"/>
+      <c r="I113" s="23"/>
+      <c r="J113" s="23"/>
+      <c r="K113" s="23"/>
+      <c r="L113" s="23"/>
+      <c r="M113" s="23"/>
+      <c r="N113" s="23"/>
+      <c r="O113" s="25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15">
+      <c r="A114" s="20"/>
+      <c r="B114" s="20"/>
+      <c r="C114" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D114" s="22">
+        <v>0.401388888888889</v>
+      </c>
+      <c r="E114" s="25">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="F114" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="G114" s="23"/>
+      <c r="H114" s="23"/>
+      <c r="I114" s="23"/>
+      <c r="J114" s="23"/>
+      <c r="K114" s="23"/>
+      <c r="L114" s="23"/>
+      <c r="M114" s="23"/>
+      <c r="N114" s="23"/>
+      <c r="O114" s="25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15">
+      <c r="A115" s="20"/>
+      <c r="B115" s="20"/>
+      <c r="C115" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D115" s="25">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="E115" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F115" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="G115" s="26"/>
+      <c r="H115" s="26"/>
+      <c r="I115" s="26"/>
+      <c r="J115" s="26"/>
+      <c r="K115" s="26"/>
+      <c r="L115" s="26"/>
+      <c r="M115" s="26"/>
+      <c r="N115" s="26"/>
+      <c r="O115" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15">
+      <c r="A116" s="20"/>
+      <c r="B116" s="20"/>
+      <c r="C116" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D116" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E116" s="25">
+        <v>0.472222222222222</v>
+      </c>
+      <c r="F116" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="G116" s="26"/>
+      <c r="H116" s="26"/>
+      <c r="I116" s="26"/>
+      <c r="J116" s="26"/>
+      <c r="K116" s="26"/>
+      <c r="L116" s="26"/>
+      <c r="M116" s="26"/>
+      <c r="N116" s="26"/>
+      <c r="O116" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15">
+      <c r="A117" s="20"/>
+      <c r="B117" s="20"/>
+      <c r="C117" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D117" s="25">
+        <v>0.472222222222222</v>
+      </c>
+      <c r="E117" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F117" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="G117" s="26"/>
+      <c r="H117" s="26"/>
+      <c r="I117" s="26"/>
+      <c r="J117" s="26"/>
+      <c r="K117" s="26"/>
+      <c r="L117" s="26"/>
+      <c r="M117" s="26"/>
+      <c r="N117" s="26"/>
+      <c r="O117" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15">
+      <c r="A118" s="20"/>
+      <c r="B118" s="20"/>
+      <c r="C118" s="24"/>
+      <c r="D118" s="25"/>
+      <c r="E118" s="25"/>
+      <c r="F118" s="26"/>
+      <c r="G118" s="26"/>
+      <c r="H118" s="26"/>
+      <c r="I118" s="26"/>
+      <c r="J118" s="26"/>
+      <c r="K118" s="26"/>
+      <c r="L118" s="26"/>
+      <c r="M118" s="26"/>
+      <c r="N118" s="26"/>
+      <c r="O118" s="25"/>
+    </row>
+    <row r="119" spans="1:15">
+      <c r="A119" s="20"/>
+      <c r="B119" s="20"/>
+      <c r="C119" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D119" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E119" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F119" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="G119" s="26"/>
+      <c r="H119" s="26"/>
+      <c r="I119" s="26"/>
+      <c r="J119" s="26"/>
+      <c r="K119" s="26"/>
+      <c r="L119" s="26"/>
+      <c r="M119" s="26"/>
+      <c r="N119" s="26"/>
+      <c r="O119" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15">
+      <c r="A120" s="20"/>
+      <c r="B120" s="20"/>
+      <c r="C120" s="24"/>
+      <c r="D120" s="25"/>
+      <c r="E120" s="25"/>
+      <c r="F120" s="26"/>
+      <c r="G120" s="26"/>
+      <c r="H120" s="26"/>
+      <c r="I120" s="26"/>
+      <c r="J120" s="26"/>
+      <c r="K120" s="26"/>
+      <c r="L120" s="26"/>
+      <c r="M120" s="26"/>
+      <c r="N120" s="26"/>
+      <c r="O120" s="25"/>
+    </row>
+    <row r="121" spans="1:15">
+      <c r="A121" s="20"/>
+      <c r="B121" s="20"/>
+      <c r="C121" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D121" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E121" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F121" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="G121" s="26"/>
+      <c r="H121" s="26"/>
+      <c r="I121" s="26"/>
+      <c r="J121" s="26"/>
+      <c r="K121" s="26"/>
+      <c r="L121" s="26"/>
+      <c r="M121" s="26"/>
+      <c r="N121" s="26"/>
+      <c r="O121" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15">
+      <c r="A122" s="20"/>
+      <c r="B122" s="20"/>
+      <c r="C122" s="24"/>
+      <c r="D122" s="25"/>
+      <c r="E122" s="25"/>
+      <c r="F122" s="26"/>
+      <c r="G122" s="26"/>
+      <c r="H122" s="26"/>
+      <c r="I122" s="26"/>
+      <c r="J122" s="26"/>
+      <c r="K122" s="26"/>
+      <c r="L122" s="26"/>
+      <c r="M122" s="26"/>
+      <c r="N122" s="26"/>
+      <c r="O122" s="25"/>
+    </row>
+    <row r="126" spans="1:15">
+      <c r="A126" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B126" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D126" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E126" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F126" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G126" s="19"/>
+      <c r="H126" s="19"/>
+      <c r="I126" s="19"/>
+      <c r="J126" s="19"/>
+      <c r="K126" s="19"/>
+      <c r="L126" s="19"/>
+      <c r="M126" s="19"/>
+      <c r="N126" s="19"/>
+      <c r="O126" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15">
+      <c r="A127" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B127" s="20">
+        <v>45120</v>
+      </c>
+      <c r="C127" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D127" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E127" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F127" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="G127" s="26"/>
+      <c r="H127" s="26"/>
+      <c r="I127" s="26"/>
+      <c r="J127" s="26"/>
+      <c r="K127" s="26"/>
+      <c r="L127" s="26"/>
+      <c r="M127" s="26"/>
+      <c r="N127" s="26"/>
+      <c r="O127" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="128" spans="1:15">
+      <c r="A128" s="20"/>
+      <c r="B128" s="20"/>
+      <c r="C128" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D128" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E128" s="25">
+        <v>0.527777777777778</v>
+      </c>
+      <c r="F128" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="G128" s="26"/>
+      <c r="H128" s="26"/>
+      <c r="I128" s="26"/>
+      <c r="J128" s="26"/>
+      <c r="K128" s="26"/>
+      <c r="L128" s="26"/>
+      <c r="M128" s="26"/>
+      <c r="N128" s="26"/>
+      <c r="O128" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15">
+      <c r="A129" s="20"/>
+      <c r="B129" s="20"/>
+      <c r="C129" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D129" s="25">
+        <v>0.527777777777778</v>
+      </c>
+      <c r="E129" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F129" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="G129" s="26"/>
+      <c r="H129" s="26"/>
+      <c r="I129" s="26"/>
+      <c r="J129" s="26"/>
+      <c r="K129" s="26"/>
+      <c r="L129" s="26"/>
+      <c r="M129" s="26"/>
+      <c r="N129" s="26"/>
+      <c r="O129" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15">
+      <c r="A130" s="20"/>
+      <c r="B130" s="20"/>
+      <c r="C130" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D130" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E130" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F130" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="G130" s="26"/>
+      <c r="H130" s="26"/>
+      <c r="I130" s="26"/>
+      <c r="J130" s="26"/>
+      <c r="K130" s="26"/>
+      <c r="L130" s="26"/>
+      <c r="M130" s="26"/>
+      <c r="N130" s="26"/>
+      <c r="O130" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15">
+      <c r="A131" s="20"/>
+      <c r="B131" s="20"/>
+      <c r="C131" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D131" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E131" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F131" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="G131" s="26"/>
+      <c r="H131" s="26"/>
+      <c r="I131" s="26"/>
+      <c r="J131" s="26"/>
+      <c r="K131" s="26"/>
+      <c r="L131" s="26"/>
+      <c r="M131" s="26"/>
+      <c r="N131" s="26"/>
+      <c r="O131" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15">
+      <c r="A132" s="20"/>
+      <c r="B132" s="20"/>
+      <c r="C132" s="24"/>
+      <c r="D132" s="25"/>
+      <c r="E132" s="25"/>
+      <c r="F132" s="26"/>
+      <c r="G132" s="26"/>
+      <c r="H132" s="26"/>
+      <c r="I132" s="26"/>
+      <c r="J132" s="26"/>
+      <c r="K132" s="26"/>
+      <c r="L132" s="26"/>
+      <c r="M132" s="26"/>
+      <c r="N132" s="26"/>
+      <c r="O132" s="25"/>
+    </row>
+    <row r="133" spans="1:15">
+      <c r="A133" s="29"/>
+      <c r="B133" s="29"/>
+      <c r="C133" s="29"/>
+      <c r="D133" s="29"/>
+      <c r="E133" s="29"/>
+      <c r="F133" s="34"/>
+      <c r="G133" s="34"/>
+      <c r="H133" s="34"/>
+      <c r="I133" s="34"/>
+      <c r="J133" s="34"/>
+      <c r="K133" s="34"/>
+      <c r="L133" s="34"/>
+      <c r="M133" s="34"/>
+      <c r="N133" s="34"/>
+      <c r="O133" s="29"/>
+    </row>
+    <row r="134" spans="1:15">
+      <c r="A134" s="29"/>
+      <c r="B134" s="29"/>
+      <c r="C134" s="29"/>
+      <c r="D134" s="29"/>
+      <c r="E134" s="29"/>
+      <c r="F134" s="34"/>
+      <c r="G134" s="34"/>
+      <c r="H134" s="34"/>
+      <c r="I134" s="34"/>
+      <c r="J134" s="34"/>
+      <c r="K134" s="34"/>
+      <c r="L134" s="34"/>
+      <c r="M134" s="34"/>
+      <c r="N134" s="34"/>
+      <c r="O134" s="29"/>
+    </row>
+    <row r="135" spans="1:15">
+      <c r="A135" s="29"/>
+      <c r="B135" s="29"/>
+      <c r="C135" s="29"/>
+      <c r="D135" s="29"/>
+      <c r="E135" s="29"/>
+      <c r="F135" s="34"/>
+      <c r="G135" s="34"/>
+      <c r="H135" s="34"/>
+      <c r="I135" s="34"/>
+      <c r="J135" s="34"/>
+      <c r="K135" s="34"/>
+      <c r="L135" s="34"/>
+      <c r="M135" s="34"/>
+      <c r="N135" s="34"/>
+      <c r="O135" s="29"/>
+    </row>
+    <row r="136" spans="1:15">
+      <c r="A136" s="29"/>
+      <c r="B136" s="29"/>
+      <c r="C136" s="29"/>
+      <c r="D136" s="29"/>
+      <c r="E136" s="29"/>
+      <c r="F136" s="34"/>
+      <c r="G136" s="34"/>
+      <c r="H136" s="34"/>
+      <c r="I136" s="34"/>
+      <c r="J136" s="34"/>
+      <c r="K136" s="34"/>
+      <c r="L136" s="34"/>
+      <c r="M136" s="34"/>
+      <c r="N136" s="34"/>
+      <c r="O136" s="29"/>
+    </row>
+    <row r="141" spans="7:15">
+      <c r="G141" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="H141" s="26"/>
+      <c r="I141" s="26"/>
+      <c r="J141" s="26"/>
+      <c r="K141" s="26"/>
+      <c r="L141" s="26"/>
+      <c r="M141" s="26"/>
+      <c r="N141" s="26"/>
+      <c r="O141" s="26"/>
+    </row>
+    <row r="143" spans="7:15">
+      <c r="G143" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="H143" s="26"/>
+      <c r="I143" s="26"/>
+      <c r="J143" s="26"/>
+      <c r="K143" s="26"/>
+      <c r="L143" s="26"/>
+      <c r="M143" s="26"/>
+      <c r="N143" s="26"/>
+      <c r="O143" s="26"/>
+    </row>
   </sheetData>
-  <mergeCells count="63">
+  <mergeCells count="133">
     <mergeCell ref="C7:N7"/>
     <mergeCell ref="C13:N13"/>
     <mergeCell ref="F19:N19"/>
@@ -2858,6 +4257,37 @@
     <mergeCell ref="F70:N70"/>
     <mergeCell ref="F71:N71"/>
     <mergeCell ref="F72:N72"/>
+    <mergeCell ref="C75:O75"/>
+    <mergeCell ref="C81:O81"/>
+    <mergeCell ref="F87:N87"/>
+    <mergeCell ref="F88:N88"/>
+    <mergeCell ref="F89:N89"/>
+    <mergeCell ref="F90:N90"/>
+    <mergeCell ref="F91:N91"/>
+    <mergeCell ref="F94:N94"/>
+    <mergeCell ref="F95:N95"/>
+    <mergeCell ref="F99:N99"/>
+    <mergeCell ref="F100:N100"/>
+    <mergeCell ref="F101:N101"/>
+    <mergeCell ref="F102:N102"/>
+    <mergeCell ref="F103:N103"/>
+    <mergeCell ref="F104:N104"/>
+    <mergeCell ref="F105:N105"/>
+    <mergeCell ref="F106:N106"/>
+    <mergeCell ref="F107:N107"/>
+    <mergeCell ref="F108:N108"/>
+    <mergeCell ref="F112:N112"/>
+    <mergeCell ref="F113:N113"/>
+    <mergeCell ref="F114:N114"/>
+    <mergeCell ref="F115:N115"/>
+    <mergeCell ref="F116:N116"/>
+    <mergeCell ref="F126:N126"/>
+    <mergeCell ref="F127:N127"/>
+    <mergeCell ref="F128:N128"/>
+    <mergeCell ref="F129:N129"/>
+    <mergeCell ref="F130:N130"/>
+    <mergeCell ref="G141:O141"/>
+    <mergeCell ref="G143:O143"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A20:A27"/>
@@ -2865,6 +4295,12 @@
     <mergeCell ref="A43:A50"/>
     <mergeCell ref="A55:A63"/>
     <mergeCell ref="A67:A72"/>
+    <mergeCell ref="A76:A78"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A88:A95"/>
+    <mergeCell ref="A100:A108"/>
+    <mergeCell ref="A113:A122"/>
+    <mergeCell ref="A127:A132"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B20:B27"/>
@@ -2872,9 +4308,42 @@
     <mergeCell ref="B43:B50"/>
     <mergeCell ref="B55:B63"/>
     <mergeCell ref="B67:B72"/>
+    <mergeCell ref="B76:B78"/>
+    <mergeCell ref="B82:B84"/>
+    <mergeCell ref="B88:B95"/>
+    <mergeCell ref="B100:B108"/>
+    <mergeCell ref="B113:B122"/>
+    <mergeCell ref="B127:B132"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="C131:C132"/>
+    <mergeCell ref="D92:D93"/>
+    <mergeCell ref="D117:D118"/>
+    <mergeCell ref="D119:D120"/>
+    <mergeCell ref="D121:D122"/>
+    <mergeCell ref="D131:D132"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="E117:E118"/>
+    <mergeCell ref="E119:E120"/>
+    <mergeCell ref="E121:E122"/>
+    <mergeCell ref="E131:E132"/>
+    <mergeCell ref="O92:O93"/>
+    <mergeCell ref="O117:O118"/>
+    <mergeCell ref="O119:O120"/>
+    <mergeCell ref="O121:O122"/>
+    <mergeCell ref="O131:O132"/>
     <mergeCell ref="F2:M3"/>
     <mergeCell ref="C8:N10"/>
     <mergeCell ref="C14:N16"/>
+    <mergeCell ref="C76:O78"/>
+    <mergeCell ref="C82:O84"/>
+    <mergeCell ref="F92:N93"/>
+    <mergeCell ref="F117:N118"/>
+    <mergeCell ref="F119:N120"/>
+    <mergeCell ref="F121:N122"/>
+    <mergeCell ref="F131:N132"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
dsr 14 july 2023
df
</commit_message>
<xml_diff>
--- a/07_july_2023/July2023.xlsx
+++ b/07_july_2023/July2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="123">
   <si>
     <t>Day</t>
   </si>
@@ -343,10 +343,46 @@
     <t>notification tracker add edit modules  N tracker type N activities N tracker formula and tracker chart and test while create N edit do not occure any type of error in all modules</t>
   </si>
   <si>
-    <t>unit, unit-type</t>
-  </si>
-  <si>
-    <t>pending- coupon,-category, store,-category, merchant.ts, signup, login</t>
+    <t>wbx-5030</t>
+  </si>
+  <si>
+    <t>10m</t>
+  </si>
+  <si>
+    <t>removed touched validation in unit, unit-type, coupon form, coupon-template,coupon-category and test while create and edit do not have any error occure</t>
+  </si>
+  <si>
+    <t>1h 20m</t>
+  </si>
+  <si>
+    <t>removed touched validation in store-category,store-form, merchant sign up module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power cut </t>
+  </si>
+  <si>
+    <t>power cut and loss of time for server start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15m </t>
+  </si>
+  <si>
+    <t>wbx-5019</t>
+  </si>
+  <si>
+    <t>work on the admin &amp; merchant profile dropdown arrow should be clickable</t>
+  </si>
+  <si>
+    <t>2h 45m</t>
+  </si>
+  <si>
+    <t>LMDI-41</t>
+  </si>
+  <si>
+    <t>R&amp;D for refersh component  should be same page where we leave page data</t>
+  </si>
+  <si>
+    <t>user, community - pagination issue fixed, user, comm, annoucement - no rec issue, invite team fix</t>
   </si>
 </sst>
 </file>
@@ -354,13 +390,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="h:mm"/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="mmm/yy"/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="180" formatCode="h:mm"/>
     <numFmt numFmtId="181" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="182" formatCode="mmm/yy"/>
+    <numFmt numFmtId="182" formatCode="dd/mmm/yy"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -402,14 +438,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -420,43 +464,6 @@
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -492,16 +499,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -516,13 +545,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -570,43 +606,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -624,13 +648,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -642,37 +660,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,31 +684,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,7 +714,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -911,18 +947,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -966,6 +1010,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -983,180 +1036,163 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="182" fontId="1" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1174,7 +1210,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="4" borderId="4" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="4" borderId="4" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="4" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1186,7 +1222,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="4" borderId="7" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="4" borderId="7" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="4" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1198,7 +1234,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="4" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="2" fillId="4" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="4" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1211,22 +1247,22 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="5" borderId="12" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="5" borderId="12" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1258,6 +1294,10 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="182" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1577,10 +1617,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:P143"/>
+  <dimension ref="A2:Q151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="O137" sqref="O137"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="G154" sqref="G154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1591,6 +1631,7 @@
     <col min="4" max="4" width="12.7142857142857" customWidth="1"/>
     <col min="5" max="5" width="10.1428571428571" customWidth="1"/>
     <col min="15" max="15" width="13.7809523809524" customWidth="1"/>
+    <col min="16" max="17" width="12.8571428571429"/>
   </cols>
   <sheetData>
     <row r="2" spans="6:13">
@@ -4115,7 +4156,7 @@
       <c r="N132" s="26"/>
       <c r="O132" s="25"/>
     </row>
-    <row r="133" spans="1:15">
+    <row r="133" spans="1:8">
       <c r="A133" s="29"/>
       <c r="B133" s="29"/>
       <c r="C133" s="29"/>
@@ -4124,15 +4165,8 @@
       <c r="F133" s="34"/>
       <c r="G133" s="34"/>
       <c r="H133" s="34"/>
-      <c r="I133" s="34"/>
-      <c r="J133" s="34"/>
-      <c r="K133" s="34"/>
-      <c r="L133" s="34"/>
-      <c r="M133" s="34"/>
-      <c r="N133" s="34"/>
-      <c r="O133" s="29"/>
-    </row>
-    <row r="134" spans="1:15">
+    </row>
+    <row r="134" spans="1:8">
       <c r="A134" s="29"/>
       <c r="B134" s="29"/>
       <c r="C134" s="29"/>
@@ -4141,13 +4175,6 @@
       <c r="F134" s="34"/>
       <c r="G134" s="34"/>
       <c r="H134" s="34"/>
-      <c r="I134" s="34"/>
-      <c r="J134" s="34"/>
-      <c r="K134" s="34"/>
-      <c r="L134" s="34"/>
-      <c r="M134" s="34"/>
-      <c r="N134" s="34"/>
-      <c r="O134" s="29"/>
     </row>
     <row r="135" spans="1:15">
       <c r="A135" s="29"/>
@@ -4167,26 +4194,146 @@
       <c r="O135" s="29"/>
     </row>
     <row r="136" spans="1:15">
-      <c r="A136" s="29"/>
-      <c r="B136" s="29"/>
-      <c r="C136" s="29"/>
-      <c r="D136" s="29"/>
-      <c r="E136" s="29"/>
-      <c r="F136" s="34"/>
-      <c r="G136" s="34"/>
-      <c r="H136" s="34"/>
-      <c r="I136" s="34"/>
-      <c r="J136" s="34"/>
-      <c r="K136" s="34"/>
-      <c r="L136" s="34"/>
-      <c r="M136" s="34"/>
-      <c r="N136" s="34"/>
-      <c r="O136" s="29"/>
-    </row>
-    <row r="141" spans="7:15">
-      <c r="G141" s="26" t="s">
+      <c r="A136" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B136" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D136" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E136" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F136" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G136" s="19"/>
+      <c r="H136" s="19"/>
+      <c r="I136" s="19"/>
+      <c r="J136" s="19"/>
+      <c r="K136" s="19"/>
+      <c r="L136" s="19"/>
+      <c r="M136" s="19"/>
+      <c r="N136" s="19"/>
+      <c r="O136" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15">
+      <c r="A137" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B137" s="20">
+        <v>45121</v>
+      </c>
+      <c r="C137" s="21" t="s">
         <v>109</v>
       </c>
+      <c r="D137" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E137" s="22">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F137" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G137" s="23"/>
+      <c r="H137" s="23"/>
+      <c r="I137" s="23"/>
+      <c r="J137" s="23"/>
+      <c r="K137" s="23"/>
+      <c r="L137" s="23"/>
+      <c r="M137" s="23"/>
+      <c r="N137" s="23"/>
+      <c r="O137" s="25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15">
+      <c r="A138" s="20"/>
+      <c r="B138" s="20"/>
+      <c r="C138" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D138" s="25">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E138" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F138" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G138" s="26"/>
+      <c r="H138" s="26"/>
+      <c r="I138" s="26"/>
+      <c r="J138" s="26"/>
+      <c r="K138" s="26"/>
+      <c r="L138" s="26"/>
+      <c r="M138" s="26"/>
+      <c r="N138" s="26"/>
+      <c r="O138" s="25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15">
+      <c r="A139" s="20"/>
+      <c r="B139" s="20"/>
+      <c r="C139" s="24"/>
+      <c r="D139" s="25"/>
+      <c r="E139" s="25"/>
+      <c r="F139" s="26"/>
+      <c r="G139" s="26"/>
+      <c r="H139" s="26"/>
+      <c r="I139" s="26"/>
+      <c r="J139" s="26"/>
+      <c r="K139" s="26"/>
+      <c r="L139" s="26"/>
+      <c r="M139" s="26"/>
+      <c r="N139" s="26"/>
+      <c r="O139" s="25"/>
+    </row>
+    <row r="140" spans="1:15">
+      <c r="A140" s="20"/>
+      <c r="B140" s="20"/>
+      <c r="C140" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D140" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E140" s="25">
+        <v>0.520833333333333</v>
+      </c>
+      <c r="F140" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G140" s="26"/>
+      <c r="H140" s="26"/>
+      <c r="I140" s="26"/>
+      <c r="J140" s="26"/>
+      <c r="K140" s="26"/>
+      <c r="L140" s="26"/>
+      <c r="M140" s="26"/>
+      <c r="N140" s="26"/>
+      <c r="O140" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15">
+      <c r="A141" s="20"/>
+      <c r="B141" s="20"/>
+      <c r="C141" s="24"/>
+      <c r="D141" s="25"/>
+      <c r="E141" s="25"/>
+      <c r="F141" s="26"/>
+      <c r="G141" s="26"/>
       <c r="H141" s="26"/>
       <c r="I141" s="26"/>
       <c r="J141" s="26"/>
@@ -4194,23 +4341,136 @@
       <c r="L141" s="26"/>
       <c r="M141" s="26"/>
       <c r="N141" s="26"/>
-      <c r="O141" s="26"/>
-    </row>
-    <row r="143" spans="7:15">
-      <c r="G143" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="H143" s="26"/>
-      <c r="I143" s="26"/>
-      <c r="J143" s="26"/>
-      <c r="K143" s="26"/>
-      <c r="L143" s="26"/>
-      <c r="M143" s="26"/>
-      <c r="N143" s="26"/>
-      <c r="O143" s="26"/>
+      <c r="O141" s="25"/>
+    </row>
+    <row r="142" spans="1:17">
+      <c r="A142" s="20"/>
+      <c r="B142" s="20"/>
+      <c r="C142" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D142" s="25">
+        <v>0.520833333333333</v>
+      </c>
+      <c r="E142" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F142" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="G142" s="23"/>
+      <c r="H142" s="23"/>
+      <c r="I142" s="23"/>
+      <c r="J142" s="23"/>
+      <c r="K142" s="23"/>
+      <c r="L142" s="23"/>
+      <c r="M142" s="23"/>
+      <c r="N142" s="23"/>
+      <c r="O142" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="P142" s="38"/>
+      <c r="Q142" s="38"/>
+    </row>
+    <row r="143" spans="1:15">
+      <c r="A143" s="20"/>
+      <c r="B143" s="20"/>
+      <c r="C143" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D143" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E143" s="25">
+        <v>0.09375</v>
+      </c>
+      <c r="F143" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="G143" s="23"/>
+      <c r="H143" s="23"/>
+      <c r="I143" s="23"/>
+      <c r="J143" s="23"/>
+      <c r="K143" s="23"/>
+      <c r="L143" s="23"/>
+      <c r="M143" s="23"/>
+      <c r="N143" s="23"/>
+      <c r="O143" s="25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15">
+      <c r="A144" s="20"/>
+      <c r="B144" s="20"/>
+      <c r="C144" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D144" s="25">
+        <v>0.09375</v>
+      </c>
+      <c r="E144" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="F144" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="G144" s="26"/>
+      <c r="H144" s="26"/>
+      <c r="I144" s="26"/>
+      <c r="J144" s="26"/>
+      <c r="K144" s="26"/>
+      <c r="L144" s="26"/>
+      <c r="M144" s="26"/>
+      <c r="N144" s="26"/>
+      <c r="O144" s="25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15">
+      <c r="A145" s="37"/>
+      <c r="B145" s="37"/>
+      <c r="C145" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="D145" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E145" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F145" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G145" s="26"/>
+      <c r="H145" s="26"/>
+      <c r="I145" s="26"/>
+      <c r="J145" s="26"/>
+      <c r="K145" s="26"/>
+      <c r="L145" s="26"/>
+      <c r="M145" s="26"/>
+      <c r="N145" s="26"/>
+      <c r="O145" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="150" spans="8:8">
+      <c r="H150" s="38"/>
+    </row>
+    <row r="151" spans="8:16">
+      <c r="H151" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="I151" s="26"/>
+      <c r="J151" s="26"/>
+      <c r="K151" s="26"/>
+      <c r="L151" s="26"/>
+      <c r="M151" s="26"/>
+      <c r="N151" s="26"/>
+      <c r="O151" s="26"/>
+      <c r="P151" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="133">
+  <mergeCells count="150">
     <mergeCell ref="C7:N7"/>
     <mergeCell ref="C13:N13"/>
     <mergeCell ref="F19:N19"/>
@@ -4286,8 +4546,13 @@
     <mergeCell ref="F128:N128"/>
     <mergeCell ref="F129:N129"/>
     <mergeCell ref="F130:N130"/>
-    <mergeCell ref="G141:O141"/>
-    <mergeCell ref="G143:O143"/>
+    <mergeCell ref="F136:N136"/>
+    <mergeCell ref="F137:N137"/>
+    <mergeCell ref="F142:N142"/>
+    <mergeCell ref="F143:N143"/>
+    <mergeCell ref="F144:N144"/>
+    <mergeCell ref="F145:N145"/>
+    <mergeCell ref="H151:P151"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A20:A27"/>
@@ -4301,6 +4566,7 @@
     <mergeCell ref="A100:A108"/>
     <mergeCell ref="A113:A122"/>
     <mergeCell ref="A127:A132"/>
+    <mergeCell ref="A137:A145"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B20:B27"/>
@@ -4314,26 +4580,35 @@
     <mergeCell ref="B100:B108"/>
     <mergeCell ref="B113:B122"/>
     <mergeCell ref="B127:B132"/>
+    <mergeCell ref="B137:B145"/>
     <mergeCell ref="C92:C93"/>
     <mergeCell ref="C117:C118"/>
     <mergeCell ref="C119:C120"/>
     <mergeCell ref="C121:C122"/>
     <mergeCell ref="C131:C132"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="C140:C141"/>
     <mergeCell ref="D92:D93"/>
     <mergeCell ref="D117:D118"/>
     <mergeCell ref="D119:D120"/>
     <mergeCell ref="D121:D122"/>
     <mergeCell ref="D131:D132"/>
+    <mergeCell ref="D138:D139"/>
+    <mergeCell ref="D140:D141"/>
     <mergeCell ref="E92:E93"/>
     <mergeCell ref="E117:E118"/>
     <mergeCell ref="E119:E120"/>
     <mergeCell ref="E121:E122"/>
     <mergeCell ref="E131:E132"/>
+    <mergeCell ref="E138:E139"/>
+    <mergeCell ref="E140:E141"/>
     <mergeCell ref="O92:O93"/>
     <mergeCell ref="O117:O118"/>
     <mergeCell ref="O119:O120"/>
     <mergeCell ref="O121:O122"/>
     <mergeCell ref="O131:O132"/>
+    <mergeCell ref="O138:O139"/>
+    <mergeCell ref="O140:O141"/>
     <mergeCell ref="F2:M3"/>
     <mergeCell ref="C8:N10"/>
     <mergeCell ref="C14:N16"/>
@@ -4344,6 +4619,8 @@
     <mergeCell ref="F119:N120"/>
     <mergeCell ref="F121:N122"/>
     <mergeCell ref="F131:N132"/>
+    <mergeCell ref="F138:N139"/>
+    <mergeCell ref="F140:N141"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
30 july complete dsr extra
</commit_message>
<xml_diff>
--- a/07_july_2023/July2023.xlsx
+++ b/07_july_2023/July2023.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23325" windowHeight="9795"/>
+    <workbookView windowWidth="23145" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="189">
   <si>
     <t>Day</t>
   </si>
@@ -382,7 +382,205 @@
     <t>R&amp;D for refersh component  should be same page where we leave page data</t>
   </si>
   <si>
-    <t>user, community - pagination issue fixed, user, comm, annoucement - no rec issue, invite team fix</t>
+    <t>removed touched validation form the activities notification team N spcial sale form and raised pr and update all 5016 prs</t>
+  </si>
+  <si>
+    <t>2h 20m</t>
+  </si>
+  <si>
+    <t>wbx-5020</t>
+  </si>
+  <si>
+    <t>work on the no record found issue in user modules</t>
+  </si>
+  <si>
+    <t>40m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20m </t>
+  </si>
+  <si>
+    <t>verify the work and raised the pr of profile dropdown issue and solve git comments</t>
+  </si>
+  <si>
+    <t>work on the no record found issue in community modules and annoucement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work on the no record found issue in program module and custom field N team module </t>
+  </si>
+  <si>
+    <t>work on the no record found issue in challenge and achievements and tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work on the no record found issue in tracker type form notification form </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1h 40m </t>
+  </si>
+  <si>
+    <t>work on the no record found splash issue in all the modules referral challenge categories challenge map form special sale form unit unit type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3h </t>
+  </si>
+  <si>
+    <t>work on the team add member invite sorting issue</t>
+  </si>
+  <si>
+    <t>update the pr and rebased the pr of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work on the no record found issue in store and merchant store category </t>
+  </si>
+  <si>
+    <t>raised step by step raised pr of no record found blink issue</t>
+  </si>
+  <si>
+    <t>work on the no record found blink issue coupon category food  report abuse manage post</t>
+  </si>
+  <si>
+    <t>2h 40m</t>
+  </si>
+  <si>
+    <t>Birthday celebration of Tejas and Nidhi</t>
+  </si>
+  <si>
+    <t>30m</t>
+  </si>
+  <si>
+    <t>wbx-4721</t>
+  </si>
+  <si>
+    <t>try to solve the pagination should be on same page where we stay  after refresh</t>
+  </si>
+  <si>
+    <t>wbx-5131</t>
+  </si>
+  <si>
+    <t>wbx-5037</t>
+  </si>
+  <si>
+    <t>try to solve the search anything after redirect issue in wbx admin side</t>
+  </si>
+  <si>
+    <t>3h 15m</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>wbx-5130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10m </t>
+  </si>
+  <si>
+    <t>try to solve the search anything after redirect issue in wbx admin side used optimized method try to solve all admin side modules</t>
+  </si>
+  <si>
+    <t>3h 20m</t>
+  </si>
+  <si>
+    <t>On Halfday leave</t>
+  </si>
+  <si>
+    <t>work on the search anything on merchant side click on back button should stay listing page</t>
+  </si>
+  <si>
+    <t>work on the referral amount blink issue</t>
+  </si>
+  <si>
+    <t>work on the wrong image showing issue on header</t>
+  </si>
+  <si>
+    <t>worked on the user module for should stay same page where we leave after reload</t>
+  </si>
+  <si>
+    <t>worked on the community module for should stay same page where we leave after reload</t>
+  </si>
+  <si>
+    <t>work on the user module which is related to the pagination issue</t>
+  </si>
+  <si>
+    <t>18m</t>
+  </si>
+  <si>
+    <t>work on the community modules try to solve the and annoucement modules</t>
+  </si>
+  <si>
+    <t>2h 42m</t>
+  </si>
+  <si>
+    <t>work on the program modules which is related to the pagination load on the same page</t>
+  </si>
+  <si>
+    <t>work on the achievement and challenge modules which is related to the pagination issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">figure Out optimum solution for stay page where we leave before reload </t>
+  </si>
+  <si>
+    <t>1h 22m</t>
+  </si>
+  <si>
+    <t>work on the user module and community module for the pagiantion issues</t>
+  </si>
+  <si>
+    <t>wbx-5142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add profile image pop and setup title for delete </t>
+  </si>
+  <si>
+    <t>work on the community modules for the pagination issue which is related to reload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1h </t>
+  </si>
+  <si>
+    <t>test all the tickets on the dev server and resolve the ticket and check all scenario in ticket</t>
+  </si>
+  <si>
+    <t>wbx-5160</t>
+  </si>
+  <si>
+    <t>work on the pagination issue in annoucement and module fixed the issue  should be stay same</t>
+  </si>
+  <si>
+    <t>program and challenge and achiements page should stay on same page where we reload</t>
+  </si>
+  <si>
+    <t>work on the pagination issue where is challenge categories and challenge map</t>
+  </si>
+  <si>
+    <t>implement the stay first page features custom fields and team modules admin payment</t>
+  </si>
+  <si>
+    <t>work on tab change reload after stay same tab in user</t>
+  </si>
+  <si>
+    <t>1h 10m</t>
+  </si>
+  <si>
+    <t>wbx-5149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">work on the merchant sign page content issue in anddroid </t>
+  </si>
+  <si>
+    <t>1h 45m</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>due to power cut and server start and ineternet connectivity</t>
+  </si>
+  <si>
+    <t>work on tab change after reload the browser in community and annoucement</t>
+  </si>
+  <si>
+    <t>work on the pagination issue in spacial-sale and tab reload issue in program challenge an achie</t>
   </si>
 </sst>
 </file>
@@ -390,15 +588,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="mmm/yy"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="h:mm"/>
-    <numFmt numFmtId="181" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="182" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="180" formatCode="mmm/yy"/>
+    <numFmt numFmtId="181" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="182" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,26 +635,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -475,16 +658,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -499,22 +681,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -522,7 +690,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -544,8 +712,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -553,7 +722,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -567,13 +744,41 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -606,7 +811,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -618,13 +835,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -636,13 +877,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -654,73 +895,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -732,19 +907,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,12 +931,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -945,52 +1156,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1014,7 +1190,31 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1034,6 +1234,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1042,311 +1257,331 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="1" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="1" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="2" fillId="4" borderId="4" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="2" fillId="4" borderId="4" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="5" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="5" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="6" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="6" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="2" fillId="4" borderId="7" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="2" fillId="4" borderId="7" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="8" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="8" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="0" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="31" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="2" fillId="4" borderId="9" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="2" fillId="4" borderId="9" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="10" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="10" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="11" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="11" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="4" fillId="5" borderId="1" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="5" borderId="1" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="5" borderId="12" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="5" borderId="12" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="4" fillId="5" borderId="1" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="13" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="13" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="14" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="14" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="15" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="15" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="1" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="1" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="5" borderId="1" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="4" fillId="5" borderId="1" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="4" fillId="5" borderId="1" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1617,10 +1852,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:Q151"/>
+  <dimension ref="A1:Q283"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="G154" sqref="G154"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A269" workbookViewId="0">
+      <selection activeCell="H290" sqref="H290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1634,6 +1869,7 @@
     <col min="16" max="17" width="12.8571428571429"/>
   </cols>
   <sheetData>
+    <row r="1" customHeight="1"/>
     <row r="2" spans="6:13">
       <c r="F2" s="1">
         <v>45108</v>
@@ -4369,8 +4605,8 @@
       <c r="O142" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="P142" s="38"/>
-      <c r="Q142" s="38"/>
+      <c r="P142" s="29"/>
+      <c r="Q142" s="29"/>
     </row>
     <row r="143" spans="1:15">
       <c r="A143" s="20"/>
@@ -4427,8 +4663,8 @@
       </c>
     </row>
     <row r="145" spans="1:15">
-      <c r="A145" s="37"/>
-      <c r="B145" s="37"/>
+      <c r="A145" s="20"/>
+      <c r="B145" s="20"/>
       <c r="C145" s="24" t="s">
         <v>120</v>
       </c>
@@ -4453,24 +4689,2790 @@
         <v>59</v>
       </c>
     </row>
-    <row r="150" spans="8:8">
-      <c r="H150" s="38"/>
-    </row>
-    <row r="151" spans="8:16">
-      <c r="H151" s="26" t="s">
+    <row r="149" spans="1:15">
+      <c r="A149" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D149" s="3"/>
+      <c r="E149" s="3"/>
+      <c r="F149" s="3"/>
+      <c r="G149" s="3"/>
+      <c r="H149" s="3"/>
+      <c r="I149" s="3"/>
+      <c r="J149" s="3"/>
+      <c r="K149" s="3"/>
+      <c r="L149" s="3"/>
+      <c r="M149" s="3"/>
+      <c r="N149" s="3"/>
+      <c r="O149" s="3"/>
+    </row>
+    <row r="150" spans="1:15">
+      <c r="A150" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B150" s="7">
+        <v>45122</v>
+      </c>
+      <c r="C150" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D150" s="35"/>
+      <c r="E150" s="35"/>
+      <c r="F150" s="35"/>
+      <c r="G150" s="35"/>
+      <c r="H150" s="35"/>
+      <c r="I150" s="35"/>
+      <c r="J150" s="35"/>
+      <c r="K150" s="35"/>
+      <c r="L150" s="35"/>
+      <c r="M150" s="35"/>
+      <c r="N150" s="35"/>
+      <c r="O150" s="35"/>
+    </row>
+    <row r="151" spans="1:15">
+      <c r="A151" s="10"/>
+      <c r="B151" s="11"/>
+      <c r="C151" s="35"/>
+      <c r="D151" s="35"/>
+      <c r="E151" s="35"/>
+      <c r="F151" s="35"/>
+      <c r="G151" s="35"/>
+      <c r="H151" s="35"/>
+      <c r="I151" s="35"/>
+      <c r="J151" s="35"/>
+      <c r="K151" s="35"/>
+      <c r="L151" s="35"/>
+      <c r="M151" s="35"/>
+      <c r="N151" s="35"/>
+      <c r="O151" s="35"/>
+    </row>
+    <row r="152" spans="1:15">
+      <c r="A152" s="14"/>
+      <c r="B152" s="15"/>
+      <c r="C152" s="35"/>
+      <c r="D152" s="35"/>
+      <c r="E152" s="35"/>
+      <c r="F152" s="35"/>
+      <c r="G152" s="35"/>
+      <c r="H152" s="35"/>
+      <c r="I152" s="35"/>
+      <c r="J152" s="35"/>
+      <c r="K152" s="35"/>
+      <c r="L152" s="35"/>
+      <c r="M152" s="35"/>
+      <c r="N152" s="35"/>
+      <c r="O152" s="35"/>
+    </row>
+    <row r="153" spans="1:14">
+      <c r="A153" s="18"/>
+      <c r="B153" s="18"/>
+      <c r="C153" s="18"/>
+      <c r="D153" s="18"/>
+      <c r="E153" s="18"/>
+      <c r="F153" s="18"/>
+      <c r="G153" s="18"/>
+      <c r="H153" s="18"/>
+      <c r="I153" s="18"/>
+      <c r="J153" s="18"/>
+      <c r="K153" s="18"/>
+      <c r="L153" s="18"/>
+      <c r="M153" s="18"/>
+      <c r="N153" s="18"/>
+    </row>
+    <row r="154" spans="1:14">
+      <c r="A154" s="18"/>
+      <c r="B154" s="18"/>
+      <c r="C154" s="18"/>
+      <c r="D154" s="18"/>
+      <c r="E154" s="18"/>
+      <c r="F154" s="18"/>
+      <c r="G154" s="18"/>
+      <c r="H154" s="18"/>
+      <c r="I154" s="18"/>
+      <c r="J154" s="18"/>
+      <c r="K154" s="18"/>
+      <c r="L154" s="18"/>
+      <c r="M154" s="18"/>
+      <c r="N154" s="18"/>
+    </row>
+    <row r="155" spans="1:15">
+      <c r="A155" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D155" s="3"/>
+      <c r="E155" s="3"/>
+      <c r="F155" s="3"/>
+      <c r="G155" s="3"/>
+      <c r="H155" s="3"/>
+      <c r="I155" s="3"/>
+      <c r="J155" s="3"/>
+      <c r="K155" s="3"/>
+      <c r="L155" s="3"/>
+      <c r="M155" s="3"/>
+      <c r="N155" s="3"/>
+      <c r="O155" s="3"/>
+    </row>
+    <row r="156" spans="1:15">
+      <c r="A156" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B156" s="7">
+        <v>45123</v>
+      </c>
+      <c r="C156" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D156" s="35"/>
+      <c r="E156" s="35"/>
+      <c r="F156" s="35"/>
+      <c r="G156" s="35"/>
+      <c r="H156" s="35"/>
+      <c r="I156" s="35"/>
+      <c r="J156" s="35"/>
+      <c r="K156" s="35"/>
+      <c r="L156" s="35"/>
+      <c r="M156" s="35"/>
+      <c r="N156" s="35"/>
+      <c r="O156" s="35"/>
+    </row>
+    <row r="157" spans="1:15">
+      <c r="A157" s="10"/>
+      <c r="B157" s="11"/>
+      <c r="C157" s="35"/>
+      <c r="D157" s="35"/>
+      <c r="E157" s="35"/>
+      <c r="F157" s="35"/>
+      <c r="G157" s="35"/>
+      <c r="H157" s="35"/>
+      <c r="I157" s="35"/>
+      <c r="J157" s="35"/>
+      <c r="K157" s="35"/>
+      <c r="L157" s="35"/>
+      <c r="M157" s="35"/>
+      <c r="N157" s="35"/>
+      <c r="O157" s="35"/>
+    </row>
+    <row r="158" spans="1:15">
+      <c r="A158" s="14"/>
+      <c r="B158" s="15"/>
+      <c r="C158" s="35"/>
+      <c r="D158" s="35"/>
+      <c r="E158" s="35"/>
+      <c r="F158" s="35"/>
+      <c r="G158" s="35"/>
+      <c r="H158" s="35"/>
+      <c r="I158" s="35"/>
+      <c r="J158" s="35"/>
+      <c r="K158" s="35"/>
+      <c r="L158" s="35"/>
+      <c r="M158" s="35"/>
+      <c r="N158" s="35"/>
+      <c r="O158" s="35"/>
+    </row>
+    <row r="159" spans="7:15">
+      <c r="G159" s="34"/>
+      <c r="H159" s="34"/>
+      <c r="I159" s="34"/>
+      <c r="J159" s="34"/>
+      <c r="K159" s="34"/>
+      <c r="L159" s="34"/>
+      <c r="M159" s="34"/>
+      <c r="N159" s="34"/>
+      <c r="O159" s="34"/>
+    </row>
+    <row r="161" spans="1:15">
+      <c r="A161" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B161" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C161" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D161" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E161" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F161" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G161" s="19"/>
+      <c r="H161" s="19"/>
+      <c r="I161" s="19"/>
+      <c r="J161" s="19"/>
+      <c r="K161" s="19"/>
+      <c r="L161" s="19"/>
+      <c r="M161" s="19"/>
+      <c r="N161" s="19"/>
+      <c r="O161" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15">
+      <c r="A162" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B162" s="20">
+        <v>45124</v>
+      </c>
+      <c r="C162" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D162" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E162" s="22">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F162" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G162" s="23"/>
+      <c r="H162" s="23"/>
+      <c r="I162" s="23"/>
+      <c r="J162" s="23"/>
+      <c r="K162" s="23"/>
+      <c r="L162" s="23"/>
+      <c r="M162" s="23"/>
+      <c r="N162" s="23"/>
+      <c r="O162" s="25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="163" spans="1:15">
+      <c r="A163" s="20"/>
+      <c r="B163" s="20"/>
+      <c r="C163" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D163" s="25">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E163" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F163" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="I151" s="26"/>
-      <c r="J151" s="26"/>
-      <c r="K151" s="26"/>
-      <c r="L151" s="26"/>
-      <c r="M151" s="26"/>
-      <c r="N151" s="26"/>
-      <c r="O151" s="26"/>
-      <c r="P151" s="26"/>
+      <c r="G163" s="26"/>
+      <c r="H163" s="26"/>
+      <c r="I163" s="26"/>
+      <c r="J163" s="26"/>
+      <c r="K163" s="26"/>
+      <c r="L163" s="26"/>
+      <c r="M163" s="26"/>
+      <c r="N163" s="26"/>
+      <c r="O163" s="25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="164" spans="1:15">
+      <c r="A164" s="20"/>
+      <c r="B164" s="20"/>
+      <c r="C164" s="24"/>
+      <c r="D164" s="25"/>
+      <c r="E164" s="25"/>
+      <c r="F164" s="26"/>
+      <c r="G164" s="26"/>
+      <c r="H164" s="26"/>
+      <c r="I164" s="26"/>
+      <c r="J164" s="26"/>
+      <c r="K164" s="26"/>
+      <c r="L164" s="26"/>
+      <c r="M164" s="26"/>
+      <c r="N164" s="26"/>
+      <c r="O164" s="25"/>
+    </row>
+    <row r="165" spans="1:15">
+      <c r="A165" s="20"/>
+      <c r="B165" s="20"/>
+      <c r="C165" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="D165" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E165" s="25">
+        <v>0.527777777777778</v>
+      </c>
+      <c r="F165" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="G165" s="26"/>
+      <c r="H165" s="26"/>
+      <c r="I165" s="26"/>
+      <c r="J165" s="26"/>
+      <c r="K165" s="26"/>
+      <c r="L165" s="26"/>
+      <c r="M165" s="26"/>
+      <c r="N165" s="26"/>
+      <c r="O165" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15">
+      <c r="A166" s="20"/>
+      <c r="B166" s="20"/>
+      <c r="C166" s="24"/>
+      <c r="D166" s="25"/>
+      <c r="E166" s="25"/>
+      <c r="F166" s="26"/>
+      <c r="G166" s="26"/>
+      <c r="H166" s="26"/>
+      <c r="I166" s="26"/>
+      <c r="J166" s="26"/>
+      <c r="K166" s="26"/>
+      <c r="L166" s="26"/>
+      <c r="M166" s="26"/>
+      <c r="N166" s="26"/>
+      <c r="O166" s="25"/>
+    </row>
+    <row r="167" spans="1:15">
+      <c r="A167" s="20"/>
+      <c r="B167" s="20"/>
+      <c r="C167" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D167" s="25">
+        <v>0.527777777777778</v>
+      </c>
+      <c r="E167" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F167" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G167" s="23"/>
+      <c r="H167" s="23"/>
+      <c r="I167" s="23"/>
+      <c r="J167" s="23"/>
+      <c r="K167" s="23"/>
+      <c r="L167" s="23"/>
+      <c r="M167" s="23"/>
+      <c r="N167" s="23"/>
+      <c r="O167" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15">
+      <c r="A168" s="20"/>
+      <c r="B168" s="20"/>
+      <c r="C168" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D168" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E168" s="25">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="F168" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="G168" s="23"/>
+      <c r="H168" s="23"/>
+      <c r="I168" s="23"/>
+      <c r="J168" s="23"/>
+      <c r="K168" s="23"/>
+      <c r="L168" s="23"/>
+      <c r="M168" s="23"/>
+      <c r="N168" s="23"/>
+      <c r="O168" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15">
+      <c r="A169" s="20"/>
+      <c r="B169" s="20"/>
+      <c r="C169" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D169" s="25">
+        <v>0.104166666666667</v>
+      </c>
+      <c r="E169" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="F169" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="G169" s="26"/>
+      <c r="H169" s="26"/>
+      <c r="I169" s="26"/>
+      <c r="J169" s="26"/>
+      <c r="K169" s="26"/>
+      <c r="L169" s="26"/>
+      <c r="M169" s="26"/>
+      <c r="N169" s="26"/>
+      <c r="O169" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="170" spans="1:15">
+      <c r="A170" s="20"/>
+      <c r="B170" s="20"/>
+      <c r="C170" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D170" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E170" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F170" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="G170" s="26"/>
+      <c r="H170" s="26"/>
+      <c r="I170" s="26"/>
+      <c r="J170" s="26"/>
+      <c r="K170" s="26"/>
+      <c r="L170" s="26"/>
+      <c r="M170" s="26"/>
+      <c r="N170" s="26"/>
+      <c r="O170" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="174" spans="1:15">
+      <c r="A174" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B174" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C174" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D174" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E174" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F174" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G174" s="19"/>
+      <c r="H174" s="19"/>
+      <c r="I174" s="19"/>
+      <c r="J174" s="19"/>
+      <c r="K174" s="19"/>
+      <c r="L174" s="19"/>
+      <c r="M174" s="19"/>
+      <c r="N174" s="19"/>
+      <c r="O174" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15">
+      <c r="A175" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B175" s="20">
+        <v>45125</v>
+      </c>
+      <c r="C175" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D175" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E175" s="22">
+        <v>0.40625</v>
+      </c>
+      <c r="F175" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G175" s="23"/>
+      <c r="H175" s="23"/>
+      <c r="I175" s="23"/>
+      <c r="J175" s="23"/>
+      <c r="K175" s="23"/>
+      <c r="L175" s="23"/>
+      <c r="M175" s="23"/>
+      <c r="N175" s="23"/>
+      <c r="O175" s="25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15">
+      <c r="A176" s="20"/>
+      <c r="B176" s="20"/>
+      <c r="C176" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="D176" s="25">
+        <v>0.40625</v>
+      </c>
+      <c r="E176" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F176" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="G176" s="26"/>
+      <c r="H176" s="26"/>
+      <c r="I176" s="26"/>
+      <c r="J176" s="26"/>
+      <c r="K176" s="26"/>
+      <c r="L176" s="26"/>
+      <c r="M176" s="26"/>
+      <c r="N176" s="26"/>
+      <c r="O176" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="177" spans="1:15">
+      <c r="A177" s="20"/>
+      <c r="B177" s="20"/>
+      <c r="C177" s="24"/>
+      <c r="D177" s="25"/>
+      <c r="E177" s="25"/>
+      <c r="F177" s="26"/>
+      <c r="G177" s="26"/>
+      <c r="H177" s="26"/>
+      <c r="I177" s="26"/>
+      <c r="J177" s="26"/>
+      <c r="K177" s="26"/>
+      <c r="L177" s="26"/>
+      <c r="M177" s="26"/>
+      <c r="N177" s="26"/>
+      <c r="O177" s="25"/>
+    </row>
+    <row r="178" spans="1:15">
+      <c r="A178" s="20"/>
+      <c r="B178" s="20"/>
+      <c r="C178" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="D178" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E178" s="25">
+        <v>0.527777777777778</v>
+      </c>
+      <c r="F178" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="G178" s="26"/>
+      <c r="H178" s="26"/>
+      <c r="I178" s="26"/>
+      <c r="J178" s="26"/>
+      <c r="K178" s="26"/>
+      <c r="L178" s="26"/>
+      <c r="M178" s="26"/>
+      <c r="N178" s="26"/>
+      <c r="O178" s="25" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="179" spans="1:15">
+      <c r="A179" s="20"/>
+      <c r="B179" s="20"/>
+      <c r="C179" s="24"/>
+      <c r="D179" s="25"/>
+      <c r="E179" s="25"/>
+      <c r="F179" s="26"/>
+      <c r="G179" s="26"/>
+      <c r="H179" s="26"/>
+      <c r="I179" s="26"/>
+      <c r="J179" s="26"/>
+      <c r="K179" s="26"/>
+      <c r="L179" s="26"/>
+      <c r="M179" s="26"/>
+      <c r="N179" s="26"/>
+      <c r="O179" s="25"/>
+    </row>
+    <row r="180" spans="1:15">
+      <c r="A180" s="20"/>
+      <c r="B180" s="20"/>
+      <c r="C180" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="D180" s="25">
+        <v>0.527777777777778</v>
+      </c>
+      <c r="E180" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F180" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G180" s="23"/>
+      <c r="H180" s="23"/>
+      <c r="I180" s="23"/>
+      <c r="J180" s="23"/>
+      <c r="K180" s="23"/>
+      <c r="L180" s="23"/>
+      <c r="M180" s="23"/>
+      <c r="N180" s="23"/>
+      <c r="O180" s="25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="181" spans="1:15">
+      <c r="A181" s="20"/>
+      <c r="B181" s="20"/>
+      <c r="C181" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="D181" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E181" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="F181" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G181" s="26"/>
+      <c r="H181" s="26"/>
+      <c r="I181" s="26"/>
+      <c r="J181" s="26"/>
+      <c r="K181" s="26"/>
+      <c r="L181" s="26"/>
+      <c r="M181" s="26"/>
+      <c r="N181" s="26"/>
+      <c r="O181" s="25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15">
+      <c r="A182" s="20"/>
+      <c r="B182" s="20"/>
+      <c r="C182" s="24"/>
+      <c r="D182" s="25"/>
+      <c r="E182" s="25"/>
+      <c r="F182" s="26"/>
+      <c r="G182" s="26"/>
+      <c r="H182" s="26"/>
+      <c r="I182" s="26"/>
+      <c r="J182" s="26"/>
+      <c r="K182" s="26"/>
+      <c r="L182" s="26"/>
+      <c r="M182" s="26"/>
+      <c r="N182" s="26"/>
+      <c r="O182" s="25"/>
+    </row>
+    <row r="183" spans="1:15">
+      <c r="A183" s="20"/>
+      <c r="B183" s="20"/>
+      <c r="C183" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D183" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E183" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="F183" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="G183" s="26"/>
+      <c r="H183" s="26"/>
+      <c r="I183" s="26"/>
+      <c r="J183" s="26"/>
+      <c r="K183" s="26"/>
+      <c r="L183" s="26"/>
+      <c r="M183" s="26"/>
+      <c r="N183" s="26"/>
+      <c r="O183" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15">
+      <c r="A184" s="20"/>
+      <c r="B184" s="20"/>
+      <c r="C184" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="D184" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="E184" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F184" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="G184" s="23"/>
+      <c r="H184" s="23"/>
+      <c r="I184" s="23"/>
+      <c r="J184" s="23"/>
+      <c r="K184" s="23"/>
+      <c r="L184" s="23"/>
+      <c r="M184" s="23"/>
+      <c r="N184" s="23"/>
+      <c r="O184" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15">
+      <c r="A187" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B187" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C187" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D187" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E187" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F187" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G187" s="19"/>
+      <c r="H187" s="19"/>
+      <c r="I187" s="19"/>
+      <c r="J187" s="19"/>
+      <c r="K187" s="19"/>
+      <c r="L187" s="19"/>
+      <c r="M187" s="19"/>
+      <c r="N187" s="19"/>
+      <c r="O187" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15">
+      <c r="A188" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B188" s="20">
+        <v>45126</v>
+      </c>
+      <c r="C188" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D188" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E188" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F188" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="G188" s="23"/>
+      <c r="H188" s="23"/>
+      <c r="I188" s="23"/>
+      <c r="J188" s="23"/>
+      <c r="K188" s="23"/>
+      <c r="L188" s="23"/>
+      <c r="M188" s="23"/>
+      <c r="N188" s="23"/>
+      <c r="O188" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15">
+      <c r="A189" s="20"/>
+      <c r="B189" s="20"/>
+      <c r="C189" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="D189" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E189" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F189" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="G189" s="26"/>
+      <c r="H189" s="26"/>
+      <c r="I189" s="26"/>
+      <c r="J189" s="26"/>
+      <c r="K189" s="26"/>
+      <c r="L189" s="26"/>
+      <c r="M189" s="26"/>
+      <c r="N189" s="26"/>
+      <c r="O189" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15">
+      <c r="A190" s="20"/>
+      <c r="B190" s="20"/>
+      <c r="C190" s="24"/>
+      <c r="D190" s="25"/>
+      <c r="E190" s="25"/>
+      <c r="F190" s="26"/>
+      <c r="G190" s="26"/>
+      <c r="H190" s="26"/>
+      <c r="I190" s="26"/>
+      <c r="J190" s="26"/>
+      <c r="K190" s="26"/>
+      <c r="L190" s="26"/>
+      <c r="M190" s="26"/>
+      <c r="N190" s="26"/>
+      <c r="O190" s="25"/>
+    </row>
+    <row r="191" spans="1:17">
+      <c r="A191" s="20"/>
+      <c r="B191" s="20"/>
+      <c r="C191" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D191" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E191" s="25">
+        <v>0.0972222222222222</v>
+      </c>
+      <c r="F191" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G191" s="23"/>
+      <c r="H191" s="23"/>
+      <c r="I191" s="23"/>
+      <c r="J191" s="23"/>
+      <c r="K191" s="23"/>
+      <c r="L191" s="23"/>
+      <c r="M191" s="23"/>
+      <c r="N191" s="23"/>
+      <c r="O191" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="P191" s="37"/>
+      <c r="Q191" s="37"/>
+    </row>
+    <row r="192" spans="1:15">
+      <c r="A192" s="20"/>
+      <c r="B192" s="20"/>
+      <c r="C192" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D192" s="25">
+        <v>0.0972222222222222</v>
+      </c>
+      <c r="E192" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="F192" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="G192" s="26"/>
+      <c r="H192" s="26"/>
+      <c r="I192" s="26"/>
+      <c r="J192" s="26"/>
+      <c r="K192" s="26"/>
+      <c r="L192" s="26"/>
+      <c r="M192" s="26"/>
+      <c r="N192" s="26"/>
+      <c r="O192" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15">
+      <c r="A193" s="20"/>
+      <c r="B193" s="20"/>
+      <c r="C193" s="24"/>
+      <c r="D193" s="25"/>
+      <c r="E193" s="25"/>
+      <c r="F193" s="26"/>
+      <c r="G193" s="26"/>
+      <c r="H193" s="26"/>
+      <c r="I193" s="26"/>
+      <c r="J193" s="26"/>
+      <c r="K193" s="26"/>
+      <c r="L193" s="26"/>
+      <c r="M193" s="26"/>
+      <c r="N193" s="26"/>
+      <c r="O193" s="25"/>
+    </row>
+    <row r="194" spans="1:15">
+      <c r="A194" s="20"/>
+      <c r="B194" s="20"/>
+      <c r="C194" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D194" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E194" s="25">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="F194" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="G194" s="26"/>
+      <c r="H194" s="26"/>
+      <c r="I194" s="26"/>
+      <c r="J194" s="26"/>
+      <c r="K194" s="26"/>
+      <c r="L194" s="26"/>
+      <c r="M194" s="26"/>
+      <c r="N194" s="26"/>
+      <c r="O194" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15">
+      <c r="A195" s="20"/>
+      <c r="B195" s="20"/>
+      <c r="C195" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="D195" s="25">
+        <v>0.229166666666667</v>
+      </c>
+      <c r="E195" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F195" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="G195" s="26"/>
+      <c r="H195" s="26"/>
+      <c r="I195" s="26"/>
+      <c r="J195" s="26"/>
+      <c r="K195" s="26"/>
+      <c r="L195" s="26"/>
+      <c r="M195" s="26"/>
+      <c r="N195" s="26"/>
+      <c r="O195" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15">
+      <c r="A196" s="29"/>
+      <c r="B196" s="29"/>
+      <c r="C196" s="29"/>
+      <c r="D196" s="29"/>
+      <c r="E196" s="29"/>
+      <c r="F196" s="34"/>
+      <c r="G196" s="34"/>
+      <c r="H196" s="34"/>
+      <c r="I196" s="34"/>
+      <c r="J196" s="34"/>
+      <c r="K196" s="34"/>
+      <c r="L196" s="34"/>
+      <c r="M196" s="34"/>
+      <c r="N196" s="34"/>
+      <c r="O196" s="29"/>
+    </row>
+    <row r="197" spans="1:15">
+      <c r="A197" s="29"/>
+      <c r="B197" s="29"/>
+      <c r="C197" s="29"/>
+      <c r="D197" s="29"/>
+      <c r="E197" s="29"/>
+      <c r="F197" s="34"/>
+      <c r="G197" s="34"/>
+      <c r="H197" s="34"/>
+      <c r="I197" s="34"/>
+      <c r="J197" s="34"/>
+      <c r="K197" s="34"/>
+      <c r="L197" s="34"/>
+      <c r="M197" s="34"/>
+      <c r="N197" s="34"/>
+      <c r="O197" s="29"/>
+    </row>
+    <row r="198" spans="1:15">
+      <c r="A198" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B198" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C198" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D198" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E198" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F198" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G198" s="19"/>
+      <c r="H198" s="19"/>
+      <c r="I198" s="19"/>
+      <c r="J198" s="19"/>
+      <c r="K198" s="19"/>
+      <c r="L198" s="19"/>
+      <c r="M198" s="19"/>
+      <c r="N198" s="19"/>
+      <c r="O198" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15">
+      <c r="A199" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B199" s="20">
+        <v>45127</v>
+      </c>
+      <c r="C199" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D199" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E199" s="22">
+        <v>0.40625</v>
+      </c>
+      <c r="F199" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G199" s="23"/>
+      <c r="H199" s="23"/>
+      <c r="I199" s="23"/>
+      <c r="J199" s="23"/>
+      <c r="K199" s="23"/>
+      <c r="L199" s="23"/>
+      <c r="M199" s="23"/>
+      <c r="N199" s="23"/>
+      <c r="O199" s="25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15">
+      <c r="A200" s="20"/>
+      <c r="B200" s="20"/>
+      <c r="C200" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="D200" s="22">
+        <v>0.40625</v>
+      </c>
+      <c r="E200" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F200" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="G200" s="26"/>
+      <c r="H200" s="26"/>
+      <c r="I200" s="26"/>
+      <c r="J200" s="26"/>
+      <c r="K200" s="26"/>
+      <c r="L200" s="26"/>
+      <c r="M200" s="26"/>
+      <c r="N200" s="26"/>
+      <c r="O200" s="25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15">
+      <c r="A201" s="20"/>
+      <c r="B201" s="20"/>
+      <c r="C201" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="D201" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E201" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="F201" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="G201" s="26"/>
+      <c r="H201" s="26"/>
+      <c r="I201" s="26"/>
+      <c r="J201" s="26"/>
+      <c r="K201" s="26"/>
+      <c r="L201" s="26"/>
+      <c r="M201" s="26"/>
+      <c r="N201" s="26"/>
+      <c r="O201" s="25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15">
+      <c r="A202" s="20"/>
+      <c r="B202" s="20"/>
+      <c r="C202" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="D202" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E202" s="25">
+        <v>0.256944444444444</v>
+      </c>
+      <c r="F202" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="G202" s="26"/>
+      <c r="H202" s="26"/>
+      <c r="I202" s="26"/>
+      <c r="J202" s="26"/>
+      <c r="K202" s="26"/>
+      <c r="L202" s="26"/>
+      <c r="M202" s="26"/>
+      <c r="N202" s="26"/>
+      <c r="O202" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15">
+      <c r="A203" s="20"/>
+      <c r="B203" s="20"/>
+      <c r="C203" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D203" s="25">
+        <v>0.256944444444444</v>
+      </c>
+      <c r="E203" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F203" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G203" s="23"/>
+      <c r="H203" s="23"/>
+      <c r="I203" s="23"/>
+      <c r="J203" s="23"/>
+      <c r="K203" s="23"/>
+      <c r="L203" s="23"/>
+      <c r="M203" s="23"/>
+      <c r="N203" s="23"/>
+      <c r="O203" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="204" spans="1:15">
+      <c r="A204" s="29"/>
+      <c r="B204" s="29"/>
+      <c r="C204" s="29"/>
+      <c r="D204" s="29"/>
+      <c r="E204" s="29"/>
+      <c r="F204" s="34"/>
+      <c r="G204" s="34"/>
+      <c r="H204" s="34"/>
+      <c r="I204" s="34"/>
+      <c r="J204" s="34"/>
+      <c r="K204" s="34"/>
+      <c r="L204" s="34"/>
+      <c r="M204" s="34"/>
+      <c r="N204" s="34"/>
+      <c r="O204" s="29"/>
+    </row>
+    <row r="205" spans="1:15">
+      <c r="A205" s="29"/>
+      <c r="B205" s="29"/>
+      <c r="C205" s="29"/>
+      <c r="D205" s="29"/>
+      <c r="E205" s="29"/>
+      <c r="F205" s="34"/>
+      <c r="G205" s="34"/>
+      <c r="H205" s="34"/>
+      <c r="I205" s="34"/>
+      <c r="J205" s="34"/>
+      <c r="K205" s="34"/>
+      <c r="L205" s="34"/>
+      <c r="M205" s="34"/>
+      <c r="N205" s="34"/>
+      <c r="O205" s="29"/>
+    </row>
+    <row r="206" spans="1:15">
+      <c r="A206" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B206" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C206" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D206" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E206" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F206" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G206" s="19"/>
+      <c r="H206" s="19"/>
+      <c r="I206" s="19"/>
+      <c r="J206" s="19"/>
+      <c r="K206" s="19"/>
+      <c r="L206" s="19"/>
+      <c r="M206" s="19"/>
+      <c r="N206" s="19"/>
+      <c r="O206" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="207" spans="1:15">
+      <c r="A207" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B207" s="20">
+        <v>45128</v>
+      </c>
+      <c r="C207" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D207" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E207" s="22">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F207" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G207" s="23"/>
+      <c r="H207" s="23"/>
+      <c r="I207" s="23"/>
+      <c r="J207" s="23"/>
+      <c r="K207" s="23"/>
+      <c r="L207" s="23"/>
+      <c r="M207" s="23"/>
+      <c r="N207" s="23"/>
+      <c r="O207" s="25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="208" spans="1:15">
+      <c r="A208" s="20"/>
+      <c r="B208" s="20"/>
+      <c r="C208" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="D208" s="25">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E208" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F208" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="G208" s="26"/>
+      <c r="H208" s="26"/>
+      <c r="I208" s="26"/>
+      <c r="J208" s="26"/>
+      <c r="K208" s="26"/>
+      <c r="L208" s="26"/>
+      <c r="M208" s="26"/>
+      <c r="N208" s="26"/>
+      <c r="O208" s="25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="209" spans="1:15">
+      <c r="A209" s="20"/>
+      <c r="B209" s="20"/>
+      <c r="C209" s="36"/>
+      <c r="D209" s="25"/>
+      <c r="E209" s="25"/>
+      <c r="F209" s="26"/>
+      <c r="G209" s="26"/>
+      <c r="H209" s="26"/>
+      <c r="I209" s="26"/>
+      <c r="J209" s="26"/>
+      <c r="K209" s="26"/>
+      <c r="L209" s="26"/>
+      <c r="M209" s="26"/>
+      <c r="N209" s="26"/>
+      <c r="O209" s="25"/>
+    </row>
+    <row r="210" spans="1:15">
+      <c r="A210" s="20"/>
+      <c r="B210" s="20"/>
+      <c r="C210" s="38"/>
+      <c r="D210" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E210" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F210" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="G210" s="26"/>
+      <c r="H210" s="26"/>
+      <c r="I210" s="26"/>
+      <c r="J210" s="26"/>
+      <c r="K210" s="26"/>
+      <c r="L210" s="26"/>
+      <c r="M210" s="26"/>
+      <c r="N210" s="26"/>
+      <c r="O210" s="40"/>
+    </row>
+    <row r="211" spans="1:15">
+      <c r="A211" s="20"/>
+      <c r="B211" s="20"/>
+      <c r="C211" s="25"/>
+      <c r="D211" s="25"/>
+      <c r="E211" s="25"/>
+      <c r="F211" s="26"/>
+      <c r="G211" s="26"/>
+      <c r="H211" s="26"/>
+      <c r="I211" s="26"/>
+      <c r="J211" s="26"/>
+      <c r="K211" s="26"/>
+      <c r="L211" s="26"/>
+      <c r="M211" s="26"/>
+      <c r="N211" s="26"/>
+      <c r="O211" s="40"/>
+    </row>
+    <row r="214" spans="1:15">
+      <c r="A214" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D214" s="3"/>
+      <c r="E214" s="3"/>
+      <c r="F214" s="3"/>
+      <c r="G214" s="3"/>
+      <c r="H214" s="3"/>
+      <c r="I214" s="3"/>
+      <c r="J214" s="3"/>
+      <c r="K214" s="3"/>
+      <c r="L214" s="3"/>
+      <c r="M214" s="3"/>
+      <c r="N214" s="3"/>
+      <c r="O214" s="3"/>
+    </row>
+    <row r="215" spans="1:15">
+      <c r="A215" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B215" s="7">
+        <v>45129</v>
+      </c>
+      <c r="C215" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D215" s="35"/>
+      <c r="E215" s="35"/>
+      <c r="F215" s="35"/>
+      <c r="G215" s="35"/>
+      <c r="H215" s="35"/>
+      <c r="I215" s="35"/>
+      <c r="J215" s="35"/>
+      <c r="K215" s="35"/>
+      <c r="L215" s="35"/>
+      <c r="M215" s="35"/>
+      <c r="N215" s="35"/>
+      <c r="O215" s="35"/>
+    </row>
+    <row r="216" spans="1:15">
+      <c r="A216" s="10"/>
+      <c r="B216" s="11"/>
+      <c r="C216" s="35"/>
+      <c r="D216" s="35"/>
+      <c r="E216" s="35"/>
+      <c r="F216" s="35"/>
+      <c r="G216" s="35"/>
+      <c r="H216" s="35"/>
+      <c r="I216" s="35"/>
+      <c r="J216" s="35"/>
+      <c r="K216" s="35"/>
+      <c r="L216" s="35"/>
+      <c r="M216" s="35"/>
+      <c r="N216" s="35"/>
+      <c r="O216" s="35"/>
+    </row>
+    <row r="217" spans="1:15">
+      <c r="A217" s="14"/>
+      <c r="B217" s="15"/>
+      <c r="C217" s="35"/>
+      <c r="D217" s="35"/>
+      <c r="E217" s="35"/>
+      <c r="F217" s="35"/>
+      <c r="G217" s="35"/>
+      <c r="H217" s="35"/>
+      <c r="I217" s="35"/>
+      <c r="J217" s="35"/>
+      <c r="K217" s="35"/>
+      <c r="L217" s="35"/>
+      <c r="M217" s="35"/>
+      <c r="N217" s="35"/>
+      <c r="O217" s="35"/>
+    </row>
+    <row r="218" spans="1:14">
+      <c r="A218" s="18"/>
+      <c r="B218" s="18"/>
+      <c r="C218" s="18"/>
+      <c r="D218" s="18"/>
+      <c r="E218" s="18"/>
+      <c r="F218" s="18"/>
+      <c r="G218" s="18"/>
+      <c r="H218" s="18"/>
+      <c r="I218" s="18"/>
+      <c r="J218" s="18"/>
+      <c r="K218" s="18"/>
+      <c r="L218" s="18"/>
+      <c r="M218" s="18"/>
+      <c r="N218" s="18"/>
+    </row>
+    <row r="219" spans="1:14">
+      <c r="A219" s="18"/>
+      <c r="B219" s="18"/>
+      <c r="C219" s="18"/>
+      <c r="D219" s="18"/>
+      <c r="E219" s="18"/>
+      <c r="F219" s="18"/>
+      <c r="G219" s="18"/>
+      <c r="H219" s="18"/>
+      <c r="I219" s="18"/>
+      <c r="J219" s="18"/>
+      <c r="K219" s="18"/>
+      <c r="L219" s="18"/>
+      <c r="M219" s="18"/>
+      <c r="N219" s="18"/>
+    </row>
+    <row r="220" spans="1:15">
+      <c r="A220" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D220" s="3"/>
+      <c r="E220" s="3"/>
+      <c r="F220" s="3"/>
+      <c r="G220" s="3"/>
+      <c r="H220" s="3"/>
+      <c r="I220" s="3"/>
+      <c r="J220" s="3"/>
+      <c r="K220" s="3"/>
+      <c r="L220" s="3"/>
+      <c r="M220" s="3"/>
+      <c r="N220" s="3"/>
+      <c r="O220" s="3"/>
+    </row>
+    <row r="221" spans="1:15">
+      <c r="A221" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B221" s="7">
+        <v>45130</v>
+      </c>
+      <c r="C221" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D221" s="35"/>
+      <c r="E221" s="35"/>
+      <c r="F221" s="35"/>
+      <c r="G221" s="35"/>
+      <c r="H221" s="35"/>
+      <c r="I221" s="35"/>
+      <c r="J221" s="35"/>
+      <c r="K221" s="35"/>
+      <c r="L221" s="35"/>
+      <c r="M221" s="35"/>
+      <c r="N221" s="35"/>
+      <c r="O221" s="35"/>
+    </row>
+    <row r="222" spans="1:15">
+      <c r="A222" s="10"/>
+      <c r="B222" s="11"/>
+      <c r="C222" s="35"/>
+      <c r="D222" s="35"/>
+      <c r="E222" s="35"/>
+      <c r="F222" s="35"/>
+      <c r="G222" s="35"/>
+      <c r="H222" s="35"/>
+      <c r="I222" s="35"/>
+      <c r="J222" s="35"/>
+      <c r="K222" s="35"/>
+      <c r="L222" s="35"/>
+      <c r="M222" s="35"/>
+      <c r="N222" s="35"/>
+      <c r="O222" s="35"/>
+    </row>
+    <row r="223" spans="1:15">
+      <c r="A223" s="14"/>
+      <c r="B223" s="15"/>
+      <c r="C223" s="35"/>
+      <c r="D223" s="35"/>
+      <c r="E223" s="35"/>
+      <c r="F223" s="35"/>
+      <c r="G223" s="35"/>
+      <c r="H223" s="35"/>
+      <c r="I223" s="35"/>
+      <c r="J223" s="35"/>
+      <c r="K223" s="35"/>
+      <c r="L223" s="35"/>
+      <c r="M223" s="35"/>
+      <c r="N223" s="35"/>
+      <c r="O223" s="35"/>
+    </row>
+    <row r="226" spans="1:15">
+      <c r="A226" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B226" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C226" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D226" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E226" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F226" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G226" s="19"/>
+      <c r="H226" s="19"/>
+      <c r="I226" s="19"/>
+      <c r="J226" s="19"/>
+      <c r="K226" s="19"/>
+      <c r="L226" s="19"/>
+      <c r="M226" s="19"/>
+      <c r="N226" s="19"/>
+      <c r="O226" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="227" spans="1:15">
+      <c r="A227" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B227" s="20">
+        <v>45131</v>
+      </c>
+      <c r="C227" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D227" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E227" s="22">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F227" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G227" s="23"/>
+      <c r="H227" s="23"/>
+      <c r="I227" s="23"/>
+      <c r="J227" s="23"/>
+      <c r="K227" s="23"/>
+      <c r="L227" s="23"/>
+      <c r="M227" s="23"/>
+      <c r="N227" s="23"/>
+      <c r="O227" s="25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="228" spans="1:15">
+      <c r="A228" s="20"/>
+      <c r="B228" s="20"/>
+      <c r="C228" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="D228" s="22">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E228" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F228" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="G228" s="26"/>
+      <c r="H228" s="26"/>
+      <c r="I228" s="26"/>
+      <c r="J228" s="26"/>
+      <c r="K228" s="26"/>
+      <c r="L228" s="26"/>
+      <c r="M228" s="26"/>
+      <c r="N228" s="26"/>
+      <c r="O228" s="25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="229" spans="1:15">
+      <c r="A229" s="20"/>
+      <c r="B229" s="20"/>
+      <c r="C229" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="D229" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E229" s="25">
+        <v>0.479166666666667</v>
+      </c>
+      <c r="F229" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="G229" s="26"/>
+      <c r="H229" s="26"/>
+      <c r="I229" s="26"/>
+      <c r="J229" s="26"/>
+      <c r="K229" s="26"/>
+      <c r="L229" s="26"/>
+      <c r="M229" s="26"/>
+      <c r="N229" s="26"/>
+      <c r="O229" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="230" spans="1:15">
+      <c r="A230" s="20"/>
+      <c r="B230" s="20"/>
+      <c r="C230" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="D230" s="25">
+        <v>0.479166666666667</v>
+      </c>
+      <c r="E230" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="F230" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="G230" s="26"/>
+      <c r="H230" s="26"/>
+      <c r="I230" s="26"/>
+      <c r="J230" s="26"/>
+      <c r="K230" s="26"/>
+      <c r="L230" s="26"/>
+      <c r="M230" s="26"/>
+      <c r="N230" s="26"/>
+      <c r="O230" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="231" spans="1:15">
+      <c r="A231" s="20"/>
+      <c r="B231" s="20"/>
+      <c r="C231" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="D231" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="E231" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F231" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="G231" s="23"/>
+      <c r="H231" s="23"/>
+      <c r="I231" s="23"/>
+      <c r="J231" s="23"/>
+      <c r="K231" s="23"/>
+      <c r="L231" s="23"/>
+      <c r="M231" s="23"/>
+      <c r="N231" s="23"/>
+      <c r="O231" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="232" spans="1:15">
+      <c r="A232" s="20"/>
+      <c r="B232" s="20"/>
+      <c r="C232" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D232" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E232" s="25">
+        <v>0.0972222222222222</v>
+      </c>
+      <c r="F232" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G232" s="23"/>
+      <c r="H232" s="23"/>
+      <c r="I232" s="23"/>
+      <c r="J232" s="23"/>
+      <c r="K232" s="23"/>
+      <c r="L232" s="23"/>
+      <c r="M232" s="23"/>
+      <c r="N232" s="23"/>
+      <c r="O232" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="233" spans="1:15">
+      <c r="A233" s="20"/>
+      <c r="B233" s="20"/>
+      <c r="C233" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D233" s="25">
+        <v>0.0972222222222222</v>
+      </c>
+      <c r="E233" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F233" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="G233" s="26"/>
+      <c r="H233" s="26"/>
+      <c r="I233" s="26"/>
+      <c r="J233" s="26"/>
+      <c r="K233" s="26"/>
+      <c r="L233" s="26"/>
+      <c r="M233" s="26"/>
+      <c r="N233" s="26"/>
+      <c r="O233" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="234" spans="1:15">
+      <c r="A234" s="20"/>
+      <c r="B234" s="20"/>
+      <c r="C234" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="D234" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E234" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F234" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="G234" s="26"/>
+      <c r="H234" s="26"/>
+      <c r="I234" s="26"/>
+      <c r="J234" s="26"/>
+      <c r="K234" s="26"/>
+      <c r="L234" s="26"/>
+      <c r="M234" s="26"/>
+      <c r="N234" s="26"/>
+      <c r="O234" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="237" spans="1:15">
+      <c r="A237" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B237" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C237" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D237" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E237" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F237" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G237" s="19"/>
+      <c r="H237" s="19"/>
+      <c r="I237" s="19"/>
+      <c r="J237" s="19"/>
+      <c r="K237" s="19"/>
+      <c r="L237" s="19"/>
+      <c r="M237" s="19"/>
+      <c r="N237" s="19"/>
+      <c r="O237" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="238" spans="1:15">
+      <c r="A238" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B238" s="20">
+        <v>45132</v>
+      </c>
+      <c r="C238" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D238" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E238" s="25">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="F238" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="G238" s="23"/>
+      <c r="H238" s="23"/>
+      <c r="I238" s="23"/>
+      <c r="J238" s="23"/>
+      <c r="K238" s="23"/>
+      <c r="L238" s="23"/>
+      <c r="M238" s="23"/>
+      <c r="N238" s="23"/>
+      <c r="O238" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="239" spans="1:15">
+      <c r="A239" s="20"/>
+      <c r="B239" s="20"/>
+      <c r="C239" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D239" s="25">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="E239" s="25">
+        <v>0.429166666666667</v>
+      </c>
+      <c r="F239" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G239" s="23"/>
+      <c r="H239" s="23"/>
+      <c r="I239" s="23"/>
+      <c r="J239" s="23"/>
+      <c r="K239" s="23"/>
+      <c r="L239" s="23"/>
+      <c r="M239" s="23"/>
+      <c r="N239" s="23"/>
+      <c r="O239" s="25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="240" spans="1:15">
+      <c r="A240" s="20"/>
+      <c r="B240" s="20"/>
+      <c r="C240" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D240" s="25">
+        <v>0.429166666666667</v>
+      </c>
+      <c r="E240" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F240" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G240" s="26"/>
+      <c r="H240" s="26"/>
+      <c r="I240" s="26"/>
+      <c r="J240" s="26"/>
+      <c r="K240" s="26"/>
+      <c r="L240" s="26"/>
+      <c r="M240" s="26"/>
+      <c r="N240" s="26"/>
+      <c r="O240" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="241" spans="1:15">
+      <c r="A241" s="20"/>
+      <c r="B241" s="20"/>
+      <c r="C241" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D241" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E241" s="25">
+        <v>0.0972222222222222</v>
+      </c>
+      <c r="F241" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G241" s="23"/>
+      <c r="H241" s="23"/>
+      <c r="I241" s="23"/>
+      <c r="J241" s="23"/>
+      <c r="K241" s="23"/>
+      <c r="L241" s="23"/>
+      <c r="M241" s="23"/>
+      <c r="N241" s="23"/>
+      <c r="O241" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="242" spans="1:15">
+      <c r="A242" s="20"/>
+      <c r="B242" s="20"/>
+      <c r="C242" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D242" s="25">
+        <v>0.0972222222222222</v>
+      </c>
+      <c r="E242" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F242" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="G242" s="23"/>
+      <c r="H242" s="23"/>
+      <c r="I242" s="23"/>
+      <c r="J242" s="23"/>
+      <c r="K242" s="23"/>
+      <c r="L242" s="23"/>
+      <c r="M242" s="23"/>
+      <c r="N242" s="23"/>
+      <c r="O242" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="243" spans="1:15">
+      <c r="A243" s="20"/>
+      <c r="B243" s="20"/>
+      <c r="C243" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D243" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E243" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F243" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G243" s="23"/>
+      <c r="H243" s="23"/>
+      <c r="I243" s="23"/>
+      <c r="J243" s="23"/>
+      <c r="K243" s="23"/>
+      <c r="L243" s="23"/>
+      <c r="M243" s="23"/>
+      <c r="N243" s="23"/>
+      <c r="O243" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="246" spans="1:15">
+      <c r="A246" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B246" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C246" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D246" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E246" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F246" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G246" s="19"/>
+      <c r="H246" s="19"/>
+      <c r="I246" s="19"/>
+      <c r="J246" s="19"/>
+      <c r="K246" s="19"/>
+      <c r="L246" s="19"/>
+      <c r="M246" s="19"/>
+      <c r="N246" s="19"/>
+      <c r="O246" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="247" spans="1:16">
+      <c r="A247" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B247" s="20">
+        <v>45133</v>
+      </c>
+      <c r="C247" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D247" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E247" s="22">
+        <v>0.401388888888889</v>
+      </c>
+      <c r="F247" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G247" s="23"/>
+      <c r="H247" s="23"/>
+      <c r="I247" s="23"/>
+      <c r="J247" s="23"/>
+      <c r="K247" s="23"/>
+      <c r="L247" s="23"/>
+      <c r="M247" s="23"/>
+      <c r="N247" s="23"/>
+      <c r="O247" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="P247">
+        <v>5130</v>
+      </c>
+    </row>
+    <row r="248" spans="1:15">
+      <c r="A248" s="20"/>
+      <c r="B248" s="20"/>
+      <c r="C248" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D248" s="22">
+        <v>0.401388888888889</v>
+      </c>
+      <c r="E248" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F248" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="G248" s="23"/>
+      <c r="H248" s="23"/>
+      <c r="I248" s="23"/>
+      <c r="J248" s="23"/>
+      <c r="K248" s="23"/>
+      <c r="L248" s="23"/>
+      <c r="M248" s="23"/>
+      <c r="N248" s="23"/>
+      <c r="O248" s="25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="249" spans="1:15">
+      <c r="A249" s="20"/>
+      <c r="B249" s="20"/>
+      <c r="C249" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D249" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E249" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F249" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="G249" s="26"/>
+      <c r="H249" s="26"/>
+      <c r="I249" s="26"/>
+      <c r="J249" s="26"/>
+      <c r="K249" s="26"/>
+      <c r="L249" s="26"/>
+      <c r="M249" s="26"/>
+      <c r="N249" s="26"/>
+      <c r="O249" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="250" spans="1:15">
+      <c r="A250" s="20"/>
+      <c r="B250" s="20"/>
+      <c r="C250" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="D250" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E250" s="25">
+        <v>0.0972222222222222</v>
+      </c>
+      <c r="F250" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G250" s="23"/>
+      <c r="H250" s="23"/>
+      <c r="I250" s="23"/>
+      <c r="J250" s="23"/>
+      <c r="K250" s="23"/>
+      <c r="L250" s="23"/>
+      <c r="M250" s="23"/>
+      <c r="N250" s="23"/>
+      <c r="O250" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="251" spans="1:15">
+      <c r="A251" s="20"/>
+      <c r="B251" s="20"/>
+      <c r="C251" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="D251" s="25">
+        <v>0.0972222222222222</v>
+      </c>
+      <c r="E251" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="F251" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="G251" s="23"/>
+      <c r="H251" s="23"/>
+      <c r="I251" s="23"/>
+      <c r="J251" s="23"/>
+      <c r="K251" s="23"/>
+      <c r="L251" s="23"/>
+      <c r="M251" s="23"/>
+      <c r="N251" s="23"/>
+      <c r="O251" s="25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="252" spans="1:15">
+      <c r="A252" s="20"/>
+      <c r="B252" s="20"/>
+      <c r="C252" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D252" s="25">
+        <v>0.208333333333333</v>
+      </c>
+      <c r="E252" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="F252" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G252" s="23"/>
+      <c r="H252" s="23"/>
+      <c r="I252" s="23"/>
+      <c r="J252" s="23"/>
+      <c r="K252" s="23"/>
+      <c r="L252" s="23"/>
+      <c r="M252" s="23"/>
+      <c r="N252" s="23"/>
+      <c r="O252" s="25" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="253" spans="1:15">
+      <c r="A253" s="20"/>
+      <c r="B253" s="20"/>
+      <c r="C253" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D253" s="25">
+        <v>0.25</v>
+      </c>
+      <c r="E253" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F253" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="G253" s="39"/>
+      <c r="H253" s="39"/>
+      <c r="I253" s="39"/>
+      <c r="J253" s="39"/>
+      <c r="K253" s="39"/>
+      <c r="L253" s="39"/>
+      <c r="M253" s="39"/>
+      <c r="N253" s="39"/>
+      <c r="O253" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="256" spans="1:15">
+      <c r="A256" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B256" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C256" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D256" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E256" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F256" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G256" s="19"/>
+      <c r="H256" s="19"/>
+      <c r="I256" s="19"/>
+      <c r="J256" s="19"/>
+      <c r="K256" s="19"/>
+      <c r="L256" s="19"/>
+      <c r="M256" s="19"/>
+      <c r="N256" s="19"/>
+      <c r="O256" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="257" spans="1:15">
+      <c r="A257" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B257" s="20">
+        <v>45134</v>
+      </c>
+      <c r="C257" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D257" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E257" s="22">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="F257" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G257" s="23"/>
+      <c r="H257" s="23"/>
+      <c r="I257" s="23"/>
+      <c r="J257" s="23"/>
+      <c r="K257" s="23"/>
+      <c r="L257" s="23"/>
+      <c r="M257" s="23"/>
+      <c r="N257" s="23"/>
+      <c r="O257" s="25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="258" spans="1:15">
+      <c r="A258" s="20"/>
+      <c r="B258" s="20"/>
+      <c r="C258" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D258" s="22">
+        <v>0.402777777777778</v>
+      </c>
+      <c r="E258" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F258" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="G258" s="23"/>
+      <c r="H258" s="23"/>
+      <c r="I258" s="23"/>
+      <c r="J258" s="23"/>
+      <c r="K258" s="23"/>
+      <c r="L258" s="23"/>
+      <c r="M258" s="23"/>
+      <c r="N258" s="23"/>
+      <c r="O258" s="25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="259" spans="1:15">
+      <c r="A259" s="20"/>
+      <c r="B259" s="20"/>
+      <c r="C259" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D259" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E259" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F259" s="26" t="s">
+        <v>177</v>
+      </c>
+      <c r="G259" s="26"/>
+      <c r="H259" s="26"/>
+      <c r="I259" s="26"/>
+      <c r="J259" s="26"/>
+      <c r="K259" s="26"/>
+      <c r="L259" s="26"/>
+      <c r="M259" s="26"/>
+      <c r="N259" s="26"/>
+      <c r="O259" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="260" spans="1:15">
+      <c r="A260" s="20"/>
+      <c r="B260" s="20"/>
+      <c r="C260" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D260" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E260" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F260" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="G260" s="23"/>
+      <c r="H260" s="23"/>
+      <c r="I260" s="23"/>
+      <c r="J260" s="23"/>
+      <c r="K260" s="23"/>
+      <c r="L260" s="23"/>
+      <c r="M260" s="23"/>
+      <c r="N260" s="23"/>
+      <c r="O260" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="261" spans="1:15">
+      <c r="A261" s="20"/>
+      <c r="B261" s="20"/>
+      <c r="C261" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D261" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E261" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F261" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="G261" s="23"/>
+      <c r="H261" s="23"/>
+      <c r="I261" s="23"/>
+      <c r="J261" s="23"/>
+      <c r="K261" s="23"/>
+      <c r="L261" s="23"/>
+      <c r="M261" s="23"/>
+      <c r="N261" s="23"/>
+      <c r="O261" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="264" spans="1:15">
+      <c r="A264" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B264" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C264" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D264" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E264" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F264" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G264" s="19"/>
+      <c r="H264" s="19"/>
+      <c r="I264" s="19"/>
+      <c r="J264" s="19"/>
+      <c r="K264" s="19"/>
+      <c r="L264" s="19"/>
+      <c r="M264" s="19"/>
+      <c r="N264" s="19"/>
+      <c r="O264" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="265" spans="1:15">
+      <c r="A265" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B265" s="20">
+        <v>45135</v>
+      </c>
+      <c r="C265" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D265" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E265" s="22">
+        <v>0.409722222222222</v>
+      </c>
+      <c r="F265" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G265" s="23"/>
+      <c r="H265" s="23"/>
+      <c r="I265" s="23"/>
+      <c r="J265" s="23"/>
+      <c r="K265" s="23"/>
+      <c r="L265" s="23"/>
+      <c r="M265" s="23"/>
+      <c r="N265" s="23"/>
+      <c r="O265" s="25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="266" spans="1:15">
+      <c r="A266" s="20"/>
+      <c r="B266" s="20"/>
+      <c r="C266" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D266" s="22">
+        <v>0.409722222222222</v>
+      </c>
+      <c r="E266" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="F266" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G266" s="23"/>
+      <c r="H266" s="23"/>
+      <c r="I266" s="23"/>
+      <c r="J266" s="23"/>
+      <c r="K266" s="23"/>
+      <c r="L266" s="23"/>
+      <c r="M266" s="23"/>
+      <c r="N266" s="23"/>
+      <c r="O266" s="25" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="267" spans="1:16">
+      <c r="A267" s="20"/>
+      <c r="B267" s="20"/>
+      <c r="C267" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="D267" s="25">
+        <v>0.458333333333333</v>
+      </c>
+      <c r="E267" s="25">
+        <v>0.53125</v>
+      </c>
+      <c r="F267" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="G267" s="26"/>
+      <c r="H267" s="26"/>
+      <c r="I267" s="26"/>
+      <c r="J267" s="26"/>
+      <c r="K267" s="26"/>
+      <c r="L267" s="26"/>
+      <c r="M267" s="26"/>
+      <c r="N267" s="26"/>
+      <c r="O267" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="P267" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="268" spans="1:15">
+      <c r="A268" s="20"/>
+      <c r="B268" s="20"/>
+      <c r="C268" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D268" s="25">
+        <v>0.53125</v>
+      </c>
+      <c r="E268" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F268" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="G268" s="23"/>
+      <c r="H268" s="23"/>
+      <c r="I268" s="23"/>
+      <c r="J268" s="23"/>
+      <c r="K268" s="23"/>
+      <c r="L268" s="23"/>
+      <c r="M268" s="23"/>
+      <c r="N268" s="23"/>
+      <c r="O268" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="269" spans="1:15">
+      <c r="A269" s="20"/>
+      <c r="B269" s="20"/>
+      <c r="C269" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D269" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E269" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F269" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="G269" s="23"/>
+      <c r="H269" s="23"/>
+      <c r="I269" s="23"/>
+      <c r="J269" s="23"/>
+      <c r="K269" s="23"/>
+      <c r="L269" s="23"/>
+      <c r="M269" s="23"/>
+      <c r="N269" s="23"/>
+      <c r="O269" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="270" spans="1:15">
+      <c r="A270" s="41"/>
+      <c r="B270" s="41"/>
+      <c r="C270" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D270" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E270" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F270" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="G270" s="23"/>
+      <c r="H270" s="23"/>
+      <c r="I270" s="23"/>
+      <c r="J270" s="23"/>
+      <c r="K270" s="23"/>
+      <c r="L270" s="23"/>
+      <c r="M270" s="23"/>
+      <c r="N270" s="23"/>
+      <c r="O270" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="274" spans="1:15">
+      <c r="A274" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B274" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C274" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D274" s="3"/>
+      <c r="E274" s="3"/>
+      <c r="F274" s="3"/>
+      <c r="G274" s="3"/>
+      <c r="H274" s="3"/>
+      <c r="I274" s="3"/>
+      <c r="J274" s="3"/>
+      <c r="K274" s="3"/>
+      <c r="L274" s="3"/>
+      <c r="M274" s="3"/>
+      <c r="N274" s="3"/>
+      <c r="O274" s="3"/>
+    </row>
+    <row r="275" spans="1:15">
+      <c r="A275" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B275" s="7">
+        <v>45136</v>
+      </c>
+      <c r="C275" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D275" s="35"/>
+      <c r="E275" s="35"/>
+      <c r="F275" s="35"/>
+      <c r="G275" s="35"/>
+      <c r="H275" s="35"/>
+      <c r="I275" s="35"/>
+      <c r="J275" s="35"/>
+      <c r="K275" s="35"/>
+      <c r="L275" s="35"/>
+      <c r="M275" s="35"/>
+      <c r="N275" s="35"/>
+      <c r="O275" s="35"/>
+    </row>
+    <row r="276" spans="1:15">
+      <c r="A276" s="10"/>
+      <c r="B276" s="11"/>
+      <c r="C276" s="35"/>
+      <c r="D276" s="35"/>
+      <c r="E276" s="35"/>
+      <c r="F276" s="35"/>
+      <c r="G276" s="35"/>
+      <c r="H276" s="35"/>
+      <c r="I276" s="35"/>
+      <c r="J276" s="35"/>
+      <c r="K276" s="35"/>
+      <c r="L276" s="35"/>
+      <c r="M276" s="35"/>
+      <c r="N276" s="35"/>
+      <c r="O276" s="35"/>
+    </row>
+    <row r="277" spans="1:15">
+      <c r="A277" s="14"/>
+      <c r="B277" s="15"/>
+      <c r="C277" s="35"/>
+      <c r="D277" s="35"/>
+      <c r="E277" s="35"/>
+      <c r="F277" s="35"/>
+      <c r="G277" s="35"/>
+      <c r="H277" s="35"/>
+      <c r="I277" s="35"/>
+      <c r="J277" s="35"/>
+      <c r="K277" s="35"/>
+      <c r="L277" s="35"/>
+      <c r="M277" s="35"/>
+      <c r="N277" s="35"/>
+      <c r="O277" s="35"/>
+    </row>
+    <row r="278" spans="1:14">
+      <c r="A278" s="18"/>
+      <c r="B278" s="18"/>
+      <c r="C278" s="18"/>
+      <c r="D278" s="18"/>
+      <c r="E278" s="18"/>
+      <c r="F278" s="18"/>
+      <c r="G278" s="18"/>
+      <c r="H278" s="18"/>
+      <c r="I278" s="18"/>
+      <c r="J278" s="18"/>
+      <c r="K278" s="18"/>
+      <c r="L278" s="18"/>
+      <c r="M278" s="18"/>
+      <c r="N278" s="18"/>
+    </row>
+    <row r="279" spans="1:14">
+      <c r="A279" s="18"/>
+      <c r="B279" s="18"/>
+      <c r="C279" s="18"/>
+      <c r="D279" s="18"/>
+      <c r="E279" s="18"/>
+      <c r="F279" s="18"/>
+      <c r="G279" s="18"/>
+      <c r="H279" s="18"/>
+      <c r="I279" s="18"/>
+      <c r="J279" s="18"/>
+      <c r="K279" s="18"/>
+      <c r="L279" s="18"/>
+      <c r="M279" s="18"/>
+      <c r="N279" s="18"/>
+    </row>
+    <row r="280" spans="1:15">
+      <c r="A280" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B280" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C280" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D280" s="3"/>
+      <c r="E280" s="3"/>
+      <c r="F280" s="3"/>
+      <c r="G280" s="3"/>
+      <c r="H280" s="3"/>
+      <c r="I280" s="3"/>
+      <c r="J280" s="3"/>
+      <c r="K280" s="3"/>
+      <c r="L280" s="3"/>
+      <c r="M280" s="3"/>
+      <c r="N280" s="3"/>
+      <c r="O280" s="3"/>
+    </row>
+    <row r="281" spans="1:15">
+      <c r="A281" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B281" s="7">
+        <v>45137</v>
+      </c>
+      <c r="C281" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D281" s="35"/>
+      <c r="E281" s="35"/>
+      <c r="F281" s="35"/>
+      <c r="G281" s="35"/>
+      <c r="H281" s="35"/>
+      <c r="I281" s="35"/>
+      <c r="J281" s="35"/>
+      <c r="K281" s="35"/>
+      <c r="L281" s="35"/>
+      <c r="M281" s="35"/>
+      <c r="N281" s="35"/>
+      <c r="O281" s="35"/>
+    </row>
+    <row r="282" spans="1:15">
+      <c r="A282" s="10"/>
+      <c r="B282" s="11"/>
+      <c r="C282" s="35"/>
+      <c r="D282" s="35"/>
+      <c r="E282" s="35"/>
+      <c r="F282" s="35"/>
+      <c r="G282" s="35"/>
+      <c r="H282" s="35"/>
+      <c r="I282" s="35"/>
+      <c r="J282" s="35"/>
+      <c r="K282" s="35"/>
+      <c r="L282" s="35"/>
+      <c r="M282" s="35"/>
+      <c r="N282" s="35"/>
+      <c r="O282" s="35"/>
+    </row>
+    <row r="283" spans="1:15">
+      <c r="A283" s="14"/>
+      <c r="B283" s="15"/>
+      <c r="C283" s="35"/>
+      <c r="D283" s="35"/>
+      <c r="E283" s="35"/>
+      <c r="F283" s="35"/>
+      <c r="G283" s="35"/>
+      <c r="H283" s="35"/>
+      <c r="I283" s="35"/>
+      <c r="J283" s="35"/>
+      <c r="K283" s="35"/>
+      <c r="L283" s="35"/>
+      <c r="M283" s="35"/>
+      <c r="N283" s="35"/>
+      <c r="O283" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="150">
+  <mergeCells count="298">
     <mergeCell ref="C7:N7"/>
     <mergeCell ref="C13:N13"/>
     <mergeCell ref="F19:N19"/>
@@ -4552,7 +7554,73 @@
     <mergeCell ref="F143:N143"/>
     <mergeCell ref="F144:N144"/>
     <mergeCell ref="F145:N145"/>
-    <mergeCell ref="H151:P151"/>
+    <mergeCell ref="C149:O149"/>
+    <mergeCell ref="C155:O155"/>
+    <mergeCell ref="F161:N161"/>
+    <mergeCell ref="F162:N162"/>
+    <mergeCell ref="F167:N167"/>
+    <mergeCell ref="F168:N168"/>
+    <mergeCell ref="F169:N169"/>
+    <mergeCell ref="F170:N170"/>
+    <mergeCell ref="F174:N174"/>
+    <mergeCell ref="F175:N175"/>
+    <mergeCell ref="F180:N180"/>
+    <mergeCell ref="F183:N183"/>
+    <mergeCell ref="F184:N184"/>
+    <mergeCell ref="F187:N187"/>
+    <mergeCell ref="F188:N188"/>
+    <mergeCell ref="F191:N191"/>
+    <mergeCell ref="F194:N194"/>
+    <mergeCell ref="F195:N195"/>
+    <mergeCell ref="F198:N198"/>
+    <mergeCell ref="F199:N199"/>
+    <mergeCell ref="F200:N200"/>
+    <mergeCell ref="F201:N201"/>
+    <mergeCell ref="F202:N202"/>
+    <mergeCell ref="F203:N203"/>
+    <mergeCell ref="F206:N206"/>
+    <mergeCell ref="F207:N207"/>
+    <mergeCell ref="C214:O214"/>
+    <mergeCell ref="C220:O220"/>
+    <mergeCell ref="F226:N226"/>
+    <mergeCell ref="F227:N227"/>
+    <mergeCell ref="F228:N228"/>
+    <mergeCell ref="F229:N229"/>
+    <mergeCell ref="F230:N230"/>
+    <mergeCell ref="F231:N231"/>
+    <mergeCell ref="F232:N232"/>
+    <mergeCell ref="F233:N233"/>
+    <mergeCell ref="F234:N234"/>
+    <mergeCell ref="F237:N237"/>
+    <mergeCell ref="F238:N238"/>
+    <mergeCell ref="F239:N239"/>
+    <mergeCell ref="F240:N240"/>
+    <mergeCell ref="F241:N241"/>
+    <mergeCell ref="F242:N242"/>
+    <mergeCell ref="F243:N243"/>
+    <mergeCell ref="F246:N246"/>
+    <mergeCell ref="F247:N247"/>
+    <mergeCell ref="F248:N248"/>
+    <mergeCell ref="F249:N249"/>
+    <mergeCell ref="F250:N250"/>
+    <mergeCell ref="F251:N251"/>
+    <mergeCell ref="F252:N252"/>
+    <mergeCell ref="F253:N253"/>
+    <mergeCell ref="F256:N256"/>
+    <mergeCell ref="F257:N257"/>
+    <mergeCell ref="F258:N258"/>
+    <mergeCell ref="F259:N259"/>
+    <mergeCell ref="F260:N260"/>
+    <mergeCell ref="F261:N261"/>
+    <mergeCell ref="F264:N264"/>
+    <mergeCell ref="F265:N265"/>
+    <mergeCell ref="F266:N266"/>
+    <mergeCell ref="F267:N267"/>
+    <mergeCell ref="F268:N268"/>
+    <mergeCell ref="F269:N269"/>
+    <mergeCell ref="F270:N270"/>
+    <mergeCell ref="C274:O274"/>
+    <mergeCell ref="C280:O280"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A20:A27"/>
@@ -4567,6 +7635,22 @@
     <mergeCell ref="A113:A122"/>
     <mergeCell ref="A127:A132"/>
     <mergeCell ref="A137:A145"/>
+    <mergeCell ref="A150:A152"/>
+    <mergeCell ref="A156:A158"/>
+    <mergeCell ref="A162:A170"/>
+    <mergeCell ref="A175:A184"/>
+    <mergeCell ref="A188:A195"/>
+    <mergeCell ref="A199:A203"/>
+    <mergeCell ref="A207:A211"/>
+    <mergeCell ref="A215:A217"/>
+    <mergeCell ref="A221:A223"/>
+    <mergeCell ref="A227:A234"/>
+    <mergeCell ref="A238:A243"/>
+    <mergeCell ref="A247:A253"/>
+    <mergeCell ref="A257:A261"/>
+    <mergeCell ref="A265:A270"/>
+    <mergeCell ref="A275:A277"/>
+    <mergeCell ref="A281:A283"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B20:B27"/>
@@ -4581,6 +7665,22 @@
     <mergeCell ref="B113:B122"/>
     <mergeCell ref="B127:B132"/>
     <mergeCell ref="B137:B145"/>
+    <mergeCell ref="B150:B152"/>
+    <mergeCell ref="B156:B158"/>
+    <mergeCell ref="B162:B170"/>
+    <mergeCell ref="B175:B184"/>
+    <mergeCell ref="B188:B195"/>
+    <mergeCell ref="B199:B203"/>
+    <mergeCell ref="B207:B211"/>
+    <mergeCell ref="B215:B217"/>
+    <mergeCell ref="B221:B223"/>
+    <mergeCell ref="B227:B234"/>
+    <mergeCell ref="B238:B243"/>
+    <mergeCell ref="B247:B253"/>
+    <mergeCell ref="B257:B261"/>
+    <mergeCell ref="B265:B270"/>
+    <mergeCell ref="B275:B277"/>
+    <mergeCell ref="B281:B283"/>
     <mergeCell ref="C92:C93"/>
     <mergeCell ref="C117:C118"/>
     <mergeCell ref="C119:C120"/>
@@ -4588,6 +7688,15 @@
     <mergeCell ref="C131:C132"/>
     <mergeCell ref="C138:C139"/>
     <mergeCell ref="C140:C141"/>
+    <mergeCell ref="C163:C164"/>
+    <mergeCell ref="C165:C166"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="C178:C179"/>
+    <mergeCell ref="C181:C182"/>
+    <mergeCell ref="C189:C190"/>
+    <mergeCell ref="C192:C193"/>
+    <mergeCell ref="C208:C209"/>
+    <mergeCell ref="C210:C211"/>
     <mergeCell ref="D92:D93"/>
     <mergeCell ref="D117:D118"/>
     <mergeCell ref="D119:D120"/>
@@ -4595,6 +7704,15 @@
     <mergeCell ref="D131:D132"/>
     <mergeCell ref="D138:D139"/>
     <mergeCell ref="D140:D141"/>
+    <mergeCell ref="D163:D164"/>
+    <mergeCell ref="D165:D166"/>
+    <mergeCell ref="D176:D177"/>
+    <mergeCell ref="D178:D179"/>
+    <mergeCell ref="D181:D182"/>
+    <mergeCell ref="D189:D190"/>
+    <mergeCell ref="D192:D193"/>
+    <mergeCell ref="D208:D209"/>
+    <mergeCell ref="D210:D211"/>
     <mergeCell ref="E92:E93"/>
     <mergeCell ref="E117:E118"/>
     <mergeCell ref="E119:E120"/>
@@ -4602,6 +7720,15 @@
     <mergeCell ref="E131:E132"/>
     <mergeCell ref="E138:E139"/>
     <mergeCell ref="E140:E141"/>
+    <mergeCell ref="E163:E164"/>
+    <mergeCell ref="E165:E166"/>
+    <mergeCell ref="E176:E177"/>
+    <mergeCell ref="E178:E179"/>
+    <mergeCell ref="E181:E182"/>
+    <mergeCell ref="E189:E190"/>
+    <mergeCell ref="E192:E193"/>
+    <mergeCell ref="E208:E209"/>
+    <mergeCell ref="E210:E211"/>
     <mergeCell ref="O92:O93"/>
     <mergeCell ref="O117:O118"/>
     <mergeCell ref="O119:O120"/>
@@ -4609,6 +7736,14 @@
     <mergeCell ref="O131:O132"/>
     <mergeCell ref="O138:O139"/>
     <mergeCell ref="O140:O141"/>
+    <mergeCell ref="O163:O164"/>
+    <mergeCell ref="O165:O166"/>
+    <mergeCell ref="O176:O177"/>
+    <mergeCell ref="O178:O179"/>
+    <mergeCell ref="O181:O182"/>
+    <mergeCell ref="O189:O190"/>
+    <mergeCell ref="O192:O193"/>
+    <mergeCell ref="O208:O209"/>
     <mergeCell ref="F2:M3"/>
     <mergeCell ref="C8:N10"/>
     <mergeCell ref="C14:N16"/>
@@ -4621,6 +7756,21 @@
     <mergeCell ref="F131:N132"/>
     <mergeCell ref="F138:N139"/>
     <mergeCell ref="F140:N141"/>
+    <mergeCell ref="C150:O152"/>
+    <mergeCell ref="C156:O158"/>
+    <mergeCell ref="F163:N164"/>
+    <mergeCell ref="F165:N166"/>
+    <mergeCell ref="F176:N177"/>
+    <mergeCell ref="F178:N179"/>
+    <mergeCell ref="F181:N182"/>
+    <mergeCell ref="F189:N190"/>
+    <mergeCell ref="F192:N193"/>
+    <mergeCell ref="F210:O211"/>
+    <mergeCell ref="F208:N209"/>
+    <mergeCell ref="C215:O217"/>
+    <mergeCell ref="C221:O223"/>
+    <mergeCell ref="C275:O277"/>
+    <mergeCell ref="C281:O283"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
31 july 2023 dsr
</commit_message>
<xml_diff>
--- a/07_july_2023/July2023.xlsx
+++ b/07_july_2023/July2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="197">
   <si>
     <t>Day</t>
   </si>
@@ -556,12 +556,18 @@
     <t>implement the stay first page features custom fields and team modules admin payment</t>
   </si>
   <si>
+    <t xml:space="preserve">Pagination implementation url </t>
+  </si>
+  <si>
     <t>work on tab change reload after stay same tab in user</t>
   </si>
   <si>
     <t>1h 10m</t>
   </si>
   <si>
+    <t xml:space="preserve">tab implementation in url </t>
+  </si>
+  <si>
     <t>wbx-5149</t>
   </si>
   <si>
@@ -581,6 +587,24 @@
   </si>
   <si>
     <t>work on the pagination issue in spacial-sale and tab reload issue in program challenge an achie</t>
+  </si>
+  <si>
+    <t>verify all working tab and raised the pr and update code</t>
+  </si>
+  <si>
+    <t>12m</t>
+  </si>
+  <si>
+    <t>worked the tab issue where stay same tab after reload in program challenge achivements and custom fields and team modules  and team</t>
+  </si>
+  <si>
+    <t>2h 48m</t>
+  </si>
+  <si>
+    <t>special sale pagination and referral pagination and notification pagination and tab switch issue</t>
+  </si>
+  <si>
+    <t>worked on the searching pagination issue not stay same page afer searching complete</t>
   </si>
 </sst>
 </file>
@@ -778,7 +802,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -812,6 +836,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB4C6E7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1292,7 +1328,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1316,16 +1352,16 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1337,86 +1373,86 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="180" fontId="1" fillId="2" borderId="1" xfId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1530,9 +1566,14 @@
     <xf numFmtId="182" fontId="4" fillId="5" borderId="1" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="4" fillId="5" borderId="1" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1852,10 +1893,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q283"/>
+  <dimension ref="A1:R292"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A269" workbookViewId="0">
-      <selection activeCell="H290" sqref="H290"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="C262" workbookViewId="0">
+      <selection activeCell="Q272" sqref="Q272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -7110,7 +7151,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="265" spans="1:15">
+    <row r="265" spans="1:18">
       <c r="A265" s="20" t="s">
         <v>56</v>
       </c>
@@ -7140,8 +7181,13 @@
       <c r="O265" s="25" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="266" spans="1:15">
+      <c r="P265" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q265" s="41"/>
+      <c r="R265" s="41"/>
+    </row>
+    <row r="266" spans="1:18">
       <c r="A266" s="20"/>
       <c r="B266" s="20"/>
       <c r="C266" s="36" t="s">
@@ -7154,7 +7200,7 @@
         <v>0.458333333333333</v>
       </c>
       <c r="F266" s="23" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G266" s="23"/>
       <c r="H266" s="23"/>
@@ -7165,14 +7211,19 @@
       <c r="M266" s="23"/>
       <c r="N266" s="23"/>
       <c r="O266" s="25" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="267" spans="1:16">
+        <v>182</v>
+      </c>
+      <c r="P266" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q266" s="42"/>
+      <c r="R266" s="43"/>
+    </row>
+    <row r="267" spans="1:18">
       <c r="A267" s="20"/>
       <c r="B267" s="20"/>
       <c r="C267" s="36" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D267" s="25">
         <v>0.458333333333333</v>
@@ -7181,7 +7232,7 @@
         <v>0.53125</v>
       </c>
       <c r="F267" s="26" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G267" s="26"/>
       <c r="H267" s="26"/>
@@ -7192,11 +7243,13 @@
       <c r="M267" s="26"/>
       <c r="N267" s="26"/>
       <c r="O267" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="P267" t="s">
-        <v>185</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="P267" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q267" s="44"/>
+      <c r="R267" s="44"/>
     </row>
     <row r="268" spans="1:15">
       <c r="A268" s="20"/>
@@ -7211,7 +7264,7 @@
         <v>0.0416666666666667</v>
       </c>
       <c r="F268" s="23" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G268" s="23"/>
       <c r="H268" s="23"/>
@@ -7238,7 +7291,7 @@
         <v>0.166666666666667</v>
       </c>
       <c r="F269" s="23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G269" s="23"/>
       <c r="H269" s="23"/>
@@ -7253,8 +7306,8 @@
       </c>
     </row>
     <row r="270" spans="1:15">
-      <c r="A270" s="41"/>
-      <c r="B270" s="41"/>
+      <c r="A270" s="20"/>
+      <c r="B270" s="20"/>
       <c r="C270" s="36" t="s">
         <v>144</v>
       </c>
@@ -7265,7 +7318,7 @@
         <v>0.270833333333333</v>
       </c>
       <c r="F270" s="23" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="G270" s="23"/>
       <c r="H270" s="23"/>
@@ -7471,8 +7524,195 @@
       <c r="N283" s="35"/>
       <c r="O283" s="35"/>
     </row>
+    <row r="286" spans="1:15">
+      <c r="A286" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B286" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C286" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D286" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E286" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F286" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G286" s="19"/>
+      <c r="H286" s="19"/>
+      <c r="I286" s="19"/>
+      <c r="J286" s="19"/>
+      <c r="K286" s="19"/>
+      <c r="L286" s="19"/>
+      <c r="M286" s="19"/>
+      <c r="N286" s="19"/>
+      <c r="O286" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="287" spans="1:15">
+      <c r="A287" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B287" s="20">
+        <v>45138</v>
+      </c>
+      <c r="C287" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D287" s="22">
+        <v>0.395833333333333</v>
+      </c>
+      <c r="E287" s="25">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="F287" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="G287" s="23"/>
+      <c r="H287" s="23"/>
+      <c r="I287" s="23"/>
+      <c r="J287" s="23"/>
+      <c r="K287" s="23"/>
+      <c r="L287" s="23"/>
+      <c r="M287" s="23"/>
+      <c r="N287" s="23"/>
+      <c r="O287" s="25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="288" spans="1:15">
+      <c r="A288" s="20"/>
+      <c r="B288" s="20"/>
+      <c r="C288" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D288" s="25">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="E288" s="25">
+        <v>0.425</v>
+      </c>
+      <c r="F288" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G288" s="23"/>
+      <c r="H288" s="23"/>
+      <c r="I288" s="23"/>
+      <c r="J288" s="23"/>
+      <c r="K288" s="23"/>
+      <c r="L288" s="23"/>
+      <c r="M288" s="23"/>
+      <c r="N288" s="23"/>
+      <c r="O288" s="25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="289" spans="1:15">
+      <c r="A289" s="20"/>
+      <c r="B289" s="20"/>
+      <c r="C289" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="D289" s="25">
+        <v>0.425</v>
+      </c>
+      <c r="E289" s="25">
+        <v>0.0416666666666667</v>
+      </c>
+      <c r="F289" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="G289" s="26"/>
+      <c r="H289" s="26"/>
+      <c r="I289" s="26"/>
+      <c r="J289" s="26"/>
+      <c r="K289" s="26"/>
+      <c r="L289" s="26"/>
+      <c r="M289" s="26"/>
+      <c r="N289" s="26"/>
+      <c r="O289" s="25" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="290" spans="1:15">
+      <c r="A290" s="20"/>
+      <c r="B290" s="20"/>
+      <c r="C290" s="38"/>
+      <c r="D290" s="25"/>
+      <c r="E290" s="25"/>
+      <c r="F290" s="26"/>
+      <c r="G290" s="26"/>
+      <c r="H290" s="26"/>
+      <c r="I290" s="26"/>
+      <c r="J290" s="26"/>
+      <c r="K290" s="26"/>
+      <c r="L290" s="26"/>
+      <c r="M290" s="26"/>
+      <c r="N290" s="26"/>
+      <c r="O290" s="25"/>
+    </row>
+    <row r="291" spans="1:15">
+      <c r="A291" s="20"/>
+      <c r="B291" s="20"/>
+      <c r="C291" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D291" s="25">
+        <v>0.0833333333333333</v>
+      </c>
+      <c r="E291" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="F291" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="G291" s="23"/>
+      <c r="H291" s="23"/>
+      <c r="I291" s="23"/>
+      <c r="J291" s="23"/>
+      <c r="K291" s="23"/>
+      <c r="L291" s="23"/>
+      <c r="M291" s="23"/>
+      <c r="N291" s="23"/>
+      <c r="O291" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="292" spans="1:15">
+      <c r="A292" s="20"/>
+      <c r="B292" s="20"/>
+      <c r="C292" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="D292" s="25">
+        <v>0.166666666666667</v>
+      </c>
+      <c r="E292" s="25">
+        <v>0.270833333333333</v>
+      </c>
+      <c r="F292" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="G292" s="23"/>
+      <c r="H292" s="23"/>
+      <c r="I292" s="23"/>
+      <c r="J292" s="23"/>
+      <c r="K292" s="23"/>
+      <c r="L292" s="23"/>
+      <c r="M292" s="23"/>
+      <c r="N292" s="23"/>
+      <c r="O292" s="25" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="298">
+  <mergeCells count="312">
     <mergeCell ref="C7:N7"/>
     <mergeCell ref="C13:N13"/>
     <mergeCell ref="F19:N19"/>
@@ -7614,13 +7854,20 @@
     <mergeCell ref="F261:N261"/>
     <mergeCell ref="F264:N264"/>
     <mergeCell ref="F265:N265"/>
+    <mergeCell ref="P265:R265"/>
     <mergeCell ref="F266:N266"/>
+    <mergeCell ref="P266:Q266"/>
     <mergeCell ref="F267:N267"/>
     <mergeCell ref="F268:N268"/>
     <mergeCell ref="F269:N269"/>
     <mergeCell ref="F270:N270"/>
     <mergeCell ref="C274:O274"/>
     <mergeCell ref="C280:O280"/>
+    <mergeCell ref="F286:N286"/>
+    <mergeCell ref="F287:N287"/>
+    <mergeCell ref="F288:N288"/>
+    <mergeCell ref="F291:N291"/>
+    <mergeCell ref="F292:N292"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A20:A27"/>
@@ -7651,6 +7898,7 @@
     <mergeCell ref="A265:A270"/>
     <mergeCell ref="A275:A277"/>
     <mergeCell ref="A281:A283"/>
+    <mergeCell ref="A287:A292"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="B20:B27"/>
@@ -7681,6 +7929,7 @@
     <mergeCell ref="B265:B270"/>
     <mergeCell ref="B275:B277"/>
     <mergeCell ref="B281:B283"/>
+    <mergeCell ref="B287:B292"/>
     <mergeCell ref="C92:C93"/>
     <mergeCell ref="C117:C118"/>
     <mergeCell ref="C119:C120"/>
@@ -7697,6 +7946,7 @@
     <mergeCell ref="C192:C193"/>
     <mergeCell ref="C208:C209"/>
     <mergeCell ref="C210:C211"/>
+    <mergeCell ref="C289:C290"/>
     <mergeCell ref="D92:D93"/>
     <mergeCell ref="D117:D118"/>
     <mergeCell ref="D119:D120"/>
@@ -7713,6 +7963,7 @@
     <mergeCell ref="D192:D193"/>
     <mergeCell ref="D208:D209"/>
     <mergeCell ref="D210:D211"/>
+    <mergeCell ref="D289:D290"/>
     <mergeCell ref="E92:E93"/>
     <mergeCell ref="E117:E118"/>
     <mergeCell ref="E119:E120"/>
@@ -7729,6 +7980,7 @@
     <mergeCell ref="E192:E193"/>
     <mergeCell ref="E208:E209"/>
     <mergeCell ref="E210:E211"/>
+    <mergeCell ref="E289:E290"/>
     <mergeCell ref="O92:O93"/>
     <mergeCell ref="O117:O118"/>
     <mergeCell ref="O119:O120"/>
@@ -7744,6 +7996,7 @@
     <mergeCell ref="O189:O190"/>
     <mergeCell ref="O192:O193"/>
     <mergeCell ref="O208:O209"/>
+    <mergeCell ref="O289:O290"/>
     <mergeCell ref="F2:M3"/>
     <mergeCell ref="C8:N10"/>
     <mergeCell ref="C14:N16"/>
@@ -7771,6 +8024,7 @@
     <mergeCell ref="C221:O223"/>
     <mergeCell ref="C275:O277"/>
     <mergeCell ref="C281:O283"/>
+    <mergeCell ref="F289:N290"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>